<commit_message>
Updated pivot tables and color coded OurGroup3 of y2000, y2010, y2018 (CCB data also added to these years to compare cardiovascular mortality) in "CA 1900-2020 Project" excel document. Within the "ccb_cause_to_100_year_cause" excel document, pivot table for all included years was created under the "ccb pivot tables" tab, and charts comparing OurGroup3 mortality between CDC WONDER and CCB data were created in the "ccb vs.cdc" tab.
</commit_message>
<xml_diff>
--- a/ccb_cause_to_100_year_cause.xlsx
+++ b/ccb_cause_to_100_year_cause.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\jaspoWork\120_years_of_death\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDDF92C-99ED-4EA7-B976-7BD6B442A0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B536998-8209-8E4B-9569-CBCB569CEFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ccb_cause_to_100_year_causes" sheetId="1" r:id="rId1"/>
+    <sheet name="ccb pivot tables" sheetId="4" r:id="rId2"/>
+    <sheet name="ccb vs. cdc" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="147" r:id="rId4"/>
+  </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="168">
   <si>
     <t>causeCode</t>
   </si>
@@ -385,9 +401,6 @@
     <t>Congenital anomalies</t>
   </si>
   <si>
-    <t>Chronic</t>
-  </si>
-  <si>
     <t>D66</t>
   </si>
   <si>
@@ -491,13 +504,49 @@
   </si>
   <si>
     <t>Code does not map</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total from ccb data</t>
+  </si>
+  <si>
+    <t>Total from cdc data</t>
+  </si>
+  <si>
+    <t>CDC WONDER</t>
+  </si>
+  <si>
+    <t>CCB Data</t>
+  </si>
+  <si>
+    <t>Sum of deaths_2000</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of deaths_2010</t>
+  </si>
+  <si>
+    <t>Sum of deaths_2018</t>
+  </si>
+  <si>
+    <t>Sum of deaths_2020</t>
+  </si>
+  <si>
+    <t>Sum of deaths_2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -505,16 +554,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -522,17 +603,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -543,6 +689,888 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="44385.688818750001" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="59" xr:uid="{1B34D8C8-DBA7-554E-AFCE-27F8C51D4782}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="C1:J60" sheet="ccb_cause_to_100_year_causes"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="OurGroup0" numFmtId="0">
+      <sharedItems count="29">
+        <s v="Tuberculosis"/>
+        <s v="Other Communicable"/>
+        <s v="Meningitis"/>
+        <s v="Pregnancy/Perinatal"/>
+        <s v="Other"/>
+        <s v="Other Cancer"/>
+        <s v="Stomach &amp; Liver+ Cancer"/>
+        <s v="Intestinal/Colorectal Cancer"/>
+        <s v="Pancreatic Cancer"/>
+        <s v="Lung+ Cancer"/>
+        <s v="Breast Cancer"/>
+        <s v="Prostate Cancer"/>
+        <s v="Brain Cancer"/>
+        <s v="Leukemia"/>
+        <s v="Hypertensive Heart Disease"/>
+        <s v="Ischemic Heart Disease"/>
+        <s v="Stroke"/>
+        <s v="Other Cardiovascular"/>
+        <s v="Diabetes"/>
+        <s v="Other Chronic"/>
+        <s v="Neurologic"/>
+        <s v="Other Gastrointestinal"/>
+        <s v="Kidney Disease"/>
+        <s v="Liver Disease"/>
+        <s v="Other Respiratory"/>
+        <s v="Motor Vehicle Accident"/>
+        <s v="Injury"/>
+        <s v="Suicide"/>
+        <s v="Homicide"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="OurGroup1" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="OurGroup3" numFmtId="0">
+      <sharedItems count="7">
+        <s v="Communicable"/>
+        <s v="Other"/>
+        <s v="Cancer"/>
+        <s v="Cardiovascular"/>
+        <s v="Other Chronic"/>
+        <s v="Injury"/>
+        <s v="Chronic" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="deaths_2000" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="36" maxValue="53593"/>
+    </cacheField>
+    <cacheField name="deaths_2010" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="40" maxValue="39133"/>
+    </cacheField>
+    <cacheField name="deaths_2018" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="40" maxValue="37099"/>
+    </cacheField>
+    <cacheField name="deaths_2019" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="16" maxValue="36197"/>
+    </cacheField>
+    <cacheField name="deaths_2020" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="29" maxValue="38777"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="59">
+  <r>
+    <x v="0"/>
+    <s v="Tuberculosis"/>
+    <x v="0"/>
+    <n v="135"/>
+    <n v="115"/>
+    <n v="103"/>
+    <n v="115"/>
+    <n v="124"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Other Communicable"/>
+    <x v="0"/>
+    <n v="1472"/>
+    <n v="744"/>
+    <n v="584"/>
+    <n v="603"/>
+    <n v="618"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Meningitis"/>
+    <x v="0"/>
+    <n v="133"/>
+    <n v="75"/>
+    <n v="79"/>
+    <n v="67"/>
+    <n v="50"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Other Communicable"/>
+    <x v="0"/>
+    <n v="36"/>
+    <n v="43"/>
+    <n v="40"/>
+    <n v="50"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Other Communicable"/>
+    <x v="0"/>
+    <n v="677"/>
+    <n v="1302"/>
+    <n v="767"/>
+    <n v="607"/>
+    <n v="602"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Other Communicable"/>
+    <x v="0"/>
+    <n v="8431"/>
+    <n v="5888"/>
+    <n v="6927"/>
+    <n v="5654"/>
+    <n v="6042"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Pregnancy/Perinatal"/>
+    <x v="1"/>
+    <n v="59"/>
+    <n v="80"/>
+    <n v="86"/>
+    <n v="68"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Pregnancy/Perinatal"/>
+    <x v="1"/>
+    <n v="1572"/>
+    <n v="1385"/>
+    <n v="1096"/>
+    <n v="1052"/>
+    <n v="941"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="COVID-19"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="30857"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Other"/>
+    <x v="1"/>
+    <n v="2150"/>
+    <n v="3261"/>
+    <n v="4127"/>
+    <n v="4255"/>
+    <n v="4636"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="801"/>
+    <n v="918"/>
+    <n v="1080"/>
+    <n v="1095"/>
+    <n v="1136"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="1154"/>
+    <n v="1243"/>
+    <n v="1356"/>
+    <n v="1358"/>
+    <n v="1313"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="Stomach &amp; Liver+ Cancer"/>
+    <x v="2"/>
+    <n v="1587"/>
+    <n v="1609"/>
+    <n v="1638"/>
+    <n v="1641"/>
+    <n v="1732"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="Intestinal/Colorectal Cancer"/>
+    <x v="2"/>
+    <n v="5248"/>
+    <n v="5224"/>
+    <n v="5449"/>
+    <n v="5497"/>
+    <n v="5520"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="Stomach &amp; Liver+ Cancer"/>
+    <x v="2"/>
+    <n v="1718"/>
+    <n v="2678"/>
+    <n v="3534"/>
+    <n v="3511"/>
+    <n v="3439"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <s v="Pancreatic Cancer"/>
+    <x v="2"/>
+    <n v="2879"/>
+    <n v="3792"/>
+    <n v="4528"/>
+    <n v="4687"/>
+    <n v="4637"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <s v="Lung+ Cancer"/>
+    <x v="2"/>
+    <n v="13697"/>
+    <n v="12899"/>
+    <n v="11073"/>
+    <n v="10710"/>
+    <n v="10360"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="1009"/>
+    <n v="1297"/>
+    <n v="1337"/>
+    <n v="1278"/>
+    <n v="1224"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <s v="Breast Cancer"/>
+    <x v="2"/>
+    <n v="4263"/>
+    <n v="4244"/>
+    <n v="4579"/>
+    <n v="4539"/>
+    <n v="4540"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="1121"/>
+    <n v="1368"/>
+    <n v="1755"/>
+    <n v="1811"/>
+    <n v="1838"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="1555"/>
+    <n v="1541"/>
+    <n v="1577"/>
+    <n v="1514"/>
+    <n v="1526"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <s v="Prostate Cancer"/>
+    <x v="2"/>
+    <n v="3008"/>
+    <n v="3045"/>
+    <n v="3707"/>
+    <n v="3615"/>
+    <n v="3811"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="1099"/>
+    <n v="1232"/>
+    <n v="1430"/>
+    <n v="1380"/>
+    <n v="1456"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="1078"/>
+    <n v="1438"/>
+    <n v="1644"/>
+    <n v="1696"/>
+    <n v="1664"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <s v="Brain Cancer"/>
+    <x v="2"/>
+    <n v="1707"/>
+    <n v="1803"/>
+    <n v="2172"/>
+    <n v="2117"/>
+    <n v="2306"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="3388"/>
+    <n v="3417"/>
+    <n v="3500"/>
+    <n v="3589"/>
+    <n v="3621"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <s v="Leukemia"/>
+    <x v="2"/>
+    <n v="2104"/>
+    <n v="2344"/>
+    <n v="2382"/>
+    <n v="2326"/>
+    <n v="2369"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Other Cancer"/>
+    <x v="2"/>
+    <n v="6020"/>
+    <n v="6332"/>
+    <n v="7207"/>
+    <n v="7110"/>
+    <n v="7296"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <s v="Hypertensive Heart Disease"/>
+    <x v="3"/>
+    <n v="5867"/>
+    <n v="8119"/>
+    <n v="11817"/>
+    <n v="12156"/>
+    <n v="13636"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <s v="Ischemic Heart Disease"/>
+    <x v="3"/>
+    <n v="53593"/>
+    <n v="39133"/>
+    <n v="37099"/>
+    <n v="36197"/>
+    <n v="38777"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <s v="Stroke"/>
+    <x v="3"/>
+    <n v="18101"/>
+    <n v="13551"/>
+    <n v="16331"/>
+    <n v="16712"/>
+    <n v="17786"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <s v="Other Cardiovascular"/>
+    <x v="3"/>
+    <n v="3607"/>
+    <n v="3148"/>
+    <n v="2946"/>
+    <n v="2844"/>
+    <n v="2808"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <s v="Other Cardiovascular"/>
+    <x v="3"/>
+    <n v="3149"/>
+    <n v="4618"/>
+    <n v="7589"/>
+    <n v="8200"/>
+    <n v="8325"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <s v="Other Cardiovascular"/>
+    <x v="3"/>
+    <n v="8668"/>
+    <n v="9416"/>
+    <n v="10752"/>
+    <n v="10665"/>
+    <n v="10979"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <s v="Diabetes"/>
+    <x v="4"/>
+    <n v="6000"/>
+    <n v="6332"/>
+    <n v="5936"/>
+    <n v="6151"/>
+    <n v="7407"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <s v="Other Chronic"/>
+    <x v="4"/>
+    <n v="1952"/>
+    <n v="2691"/>
+    <n v="3761"/>
+    <n v="3791"/>
+    <n v="4392"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <s v="Other Chronic"/>
+    <x v="4"/>
+    <n v="41"/>
+    <n v="40"/>
+    <n v="41"/>
+    <n v="16"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <s v="Neurologic"/>
+    <x v="4"/>
+    <n v="270"/>
+    <n v="212"/>
+    <n v="213"/>
+    <n v="232"/>
+    <n v="220"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <s v="Neurologic"/>
+    <x v="4"/>
+    <n v="6767"/>
+    <n v="17906"/>
+    <n v="25070"/>
+    <n v="25637"/>
+    <n v="29254"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <s v="Neurologic"/>
+    <x v="4"/>
+    <n v="3407"/>
+    <n v="4601"/>
+    <n v="6519"/>
+    <n v="7068"/>
+    <n v="7369"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <s v="Other Gastrointestinal"/>
+    <x v="1"/>
+    <n v="4579"/>
+    <n v="4209"/>
+    <n v="4504"/>
+    <n v="4673"/>
+    <n v="4815"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <s v="Kidney Disease"/>
+    <x v="1"/>
+    <n v="2127"/>
+    <n v="3871"/>
+    <n v="7545"/>
+    <n v="7777"/>
+    <n v="8707"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <s v="Liver Disease"/>
+    <x v="4"/>
+    <n v="4154"/>
+    <n v="5027"/>
+    <n v="6204"/>
+    <n v="6377"/>
+    <n v="7035"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <s v="Other Chronic"/>
+    <x v="4"/>
+    <n v="1278"/>
+    <n v="1100"/>
+    <n v="958"/>
+    <n v="992"/>
+    <n v="933"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <s v="Other Chronic"/>
+    <x v="4"/>
+    <n v="12091"/>
+    <n v="12392"/>
+    <n v="13043"/>
+    <n v="12542"/>
+    <n v="12264"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <s v="Other Chronic"/>
+    <x v="4"/>
+    <n v="555"/>
+    <n v="398"/>
+    <n v="384"/>
+    <n v="371"/>
+    <n v="435"/>
+  </r>
+  <r>
+    <x v="24"/>
+    <s v="Other Respiratory"/>
+    <x v="1"/>
+    <n v="2984"/>
+    <n v="3506"/>
+    <n v="4630"/>
+    <n v="4715"/>
+    <n v="4502"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <s v="Other Chronic"/>
+    <x v="4"/>
+    <n v="5063"/>
+    <n v="4779"/>
+    <n v="5410"/>
+    <n v="5338"/>
+    <n v="5875"/>
+  </r>
+  <r>
+    <x v="25"/>
+    <s v="Injury"/>
+    <x v="5"/>
+    <n v="4073"/>
+    <n v="2986"/>
+    <n v="4219"/>
+    <n v="4104"/>
+    <n v="4468"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <s v="Injury"/>
+    <x v="5"/>
+    <n v="2160"/>
+    <n v="3276"/>
+    <n v="5204"/>
+    <n v="6039"/>
+    <n v="8267"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <s v="Injury"/>
+    <x v="5"/>
+    <n v="56"/>
+    <n v="68"/>
+    <n v="79"/>
+    <n v="100"/>
+    <n v="110"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <s v="Injury"/>
+    <x v="5"/>
+    <n v="1251"/>
+    <n v="2059"/>
+    <n v="2586"/>
+    <n v="2802"/>
+    <n v="2780"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <s v="Injury"/>
+    <x v="5"/>
+    <n v="1745"/>
+    <n v="1642"/>
+    <n v="2205"/>
+    <n v="2155"/>
+    <n v="2053"/>
+  </r>
+  <r>
+    <x v="27"/>
+    <s v="Suicide"/>
+    <x v="5"/>
+    <n v="3113"/>
+    <n v="3805"/>
+    <n v="4423"/>
+    <n v="4343"/>
+    <n v="3992"/>
+  </r>
+  <r>
+    <x v="28"/>
+    <s v="Homicide"/>
+    <x v="5"/>
+    <n v="2151"/>
+    <n v="1961"/>
+    <n v="1967"/>
+    <n v="1849"/>
+    <n v="2392"/>
+  </r>
+  <r>
+    <x v="26"/>
+    <s v="Injury"/>
+    <x v="5"/>
+    <n v="209"/>
+    <n v="291"/>
+    <n v="250"/>
+    <n v="236"/>
+    <n v="192"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Other"/>
+    <x v="1"/>
+    <n v="1169"/>
+    <n v="870"/>
+    <n v="718"/>
+    <n v="1004"/>
+    <n v="2970"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Other"/>
+    <x v="1"/>
+    <m/>
+    <n v="337"/>
+    <m/>
+    <m/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Other"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="147" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A2:F38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="30">
+        <item x="12"/>
+        <item x="10"/>
+        <item x="18"/>
+        <item x="28"/>
+        <item x="14"/>
+        <item x="26"/>
+        <item x="7"/>
+        <item x="15"/>
+        <item x="22"/>
+        <item x="13"/>
+        <item x="23"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="25"/>
+        <item x="20"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="17"/>
+        <item x="19"/>
+        <item x="1"/>
+        <item x="21"/>
+        <item x="24"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item x="6"/>
+        <item x="16"/>
+        <item x="27"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="3"/>
+        <item m="1" x="6"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="36">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <dataFields count="5">
+    <dataField name="Sum of deaths_2000" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of deaths_2010" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of deaths_2018" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of deaths_2019" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Sum of deaths_2020" fld="7" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -824,21 +1852,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +1899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -902,7 +1931,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -934,7 +1963,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -966,7 +1995,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -998,7 +2027,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +2059,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1062,7 +2091,7 @@
         <v>6042</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1094,7 +2123,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1126,7 +2155,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1146,7 +2175,7 @@
         <v>30857</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1178,7 +2207,7 @@
         <v>4636</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1210,7 +2239,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1242,7 +2271,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1274,7 +2303,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1306,7 +2335,7 @@
         <v>5520</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1338,7 +2367,7 @@
         <v>3439</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1370,7 +2399,7 @@
         <v>4637</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1402,7 +2431,7 @@
         <v>10360</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1434,7 +2463,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1466,7 +2495,7 @@
         <v>4540</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1498,7 +2527,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1530,7 +2559,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1562,7 +2591,7 @@
         <v>3811</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -1594,7 +2623,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -1626,7 +2655,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -1658,7 +2687,7 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -1690,7 +2719,7 @@
         <v>3621</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -1722,7 +2751,7 @@
         <v>2369</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>77</v>
       </c>
@@ -1754,7 +2783,7 @@
         <v>7296</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -1786,7 +2815,7 @@
         <v>13636</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -1818,7 +2847,7 @@
         <v>38777</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -1850,7 +2879,7 @@
         <v>17786</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -1882,7 +2911,7 @@
         <v>2808</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -1914,7 +2943,7 @@
         <v>8325</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -1946,7 +2975,7 @@
         <v>10979</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -1978,7 +3007,7 @@
         <v>7407</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -2010,7 +3039,7 @@
         <v>4392</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>101</v>
       </c>
@@ -2042,7 +3071,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>103</v>
       </c>
@@ -2074,7 +3103,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -2106,7 +3135,7 @@
         <v>29254</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>108</v>
       </c>
@@ -2138,7 +3167,7 @@
         <v>7369</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>110</v>
       </c>
@@ -2170,7 +3199,7 @@
         <v>4815</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>113</v>
       </c>
@@ -2202,7 +3231,7 @@
         <v>8707</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>116</v>
       </c>
@@ -2234,7 +3263,7 @@
         <v>7035</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>119</v>
       </c>
@@ -2248,7 +3277,7 @@
         <v>98</v>
       </c>
       <c r="E45" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F45">
         <v>1278</v>
@@ -2266,12 +3295,12 @@
         <v>933</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" t="s">
         <v>122</v>
-      </c>
-      <c r="B46" t="s">
-        <v>123</v>
       </c>
       <c r="C46" t="s">
         <v>98</v>
@@ -2280,7 +3309,7 @@
         <v>98</v>
       </c>
       <c r="E46" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F46">
         <v>12091</v>
@@ -2298,12 +3327,12 @@
         <v>12264</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" t="s">
         <v>124</v>
-      </c>
-      <c r="B47" t="s">
-        <v>125</v>
       </c>
       <c r="C47" t="s">
         <v>98</v>
@@ -2312,7 +3341,7 @@
         <v>98</v>
       </c>
       <c r="E47" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F47">
         <v>555</v>
@@ -2330,18 +3359,18 @@
         <v>435</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" t="s">
         <v>126</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>127</v>
       </c>
-      <c r="C48" t="s">
-        <v>128</v>
-      </c>
       <c r="D48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E48" t="s">
         <v>27</v>
@@ -2362,12 +3391,12 @@
         <v>4502</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" t="s">
         <v>129</v>
-      </c>
-      <c r="B49" t="s">
-        <v>130</v>
       </c>
       <c r="C49" t="s">
         <v>98</v>
@@ -2376,7 +3405,7 @@
         <v>98</v>
       </c>
       <c r="E49" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="F49">
         <v>5063</v>
@@ -2394,21 +3423,21 @@
         <v>5875</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" t="s">
         <v>131</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>132</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>133</v>
       </c>
-      <c r="D50" t="s">
-        <v>134</v>
-      </c>
       <c r="E50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F50">
         <v>4073</v>
@@ -2426,21 +3455,21 @@
         <v>4468</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
         <v>135</v>
       </c>
-      <c r="B51" t="s">
-        <v>136</v>
-      </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F51">
         <v>2160</v>
@@ -2458,21 +3487,21 @@
         <v>8267</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" t="s">
         <v>137</v>
       </c>
-      <c r="B52" t="s">
-        <v>138</v>
-      </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F52">
         <v>56</v>
@@ -2490,21 +3519,21 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" t="s">
         <v>139</v>
       </c>
-      <c r="B53" t="s">
-        <v>140</v>
-      </c>
       <c r="C53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F53">
         <v>1251</v>
@@ -2522,21 +3551,21 @@
         <v>2780</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" t="s">
         <v>141</v>
       </c>
-      <c r="B54" t="s">
-        <v>142</v>
-      </c>
       <c r="C54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F54">
         <v>1745</v>
@@ -2554,21 +3583,21 @@
         <v>2053</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" t="s">
         <v>143</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>144</v>
       </c>
-      <c r="C55" t="s">
-        <v>145</v>
-      </c>
       <c r="D55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F55">
         <v>3113</v>
@@ -2586,21 +3615,21 @@
         <v>3992</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" t="s">
         <v>146</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>147</v>
       </c>
-      <c r="C56" t="s">
-        <v>148</v>
-      </c>
       <c r="D56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F56">
         <v>2151</v>
@@ -2618,21 +3647,21 @@
         <v>2392</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" t="s">
         <v>149</v>
       </c>
-      <c r="B57" t="s">
-        <v>150</v>
-      </c>
       <c r="C57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F57">
         <v>209</v>
@@ -2650,12 +3679,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" t="s">
         <v>151</v>
-      </c>
-      <c r="B58" t="s">
-        <v>152</v>
       </c>
       <c r="C58" t="s">
         <v>27</v>
@@ -2682,12 +3711,12 @@
         <v>2970</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" t="s">
         <v>153</v>
-      </c>
-      <c r="B59" t="s">
-        <v>154</v>
       </c>
       <c r="C59" t="s">
         <v>27</v>
@@ -2705,12 +3734,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" t="s">
         <v>155</v>
-      </c>
-      <c r="B60" t="s">
-        <v>156</v>
       </c>
       <c r="C60" t="s">
         <v>27</v>
@@ -2722,8 +3751,1126 @@
         <v>27</v>
       </c>
     </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3">
+        <f>SUM(F2:F60)</f>
+        <v>228281</v>
+      </c>
+      <c r="G61" s="3">
+        <f t="shared" ref="G61:J61" si="0">SUM(G2:G60)</f>
+        <v>231661</v>
+      </c>
+      <c r="H61" s="3">
+        <f t="shared" si="0"/>
+        <v>266160</v>
+      </c>
+      <c r="I61" s="3">
+        <f t="shared" si="0"/>
+        <v>267031</v>
+      </c>
+      <c r="J61" s="3">
+        <f t="shared" si="0"/>
+        <v>316540</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1">
+        <v>229697</v>
+      </c>
+      <c r="G62" s="1">
+        <v>234840</v>
+      </c>
+      <c r="H62" s="1">
+        <v>269417</v>
+      </c>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Cardiovascular">
+      <formula>NOT(ISERROR(SEARCH("Cardiovascular",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FF3F60-3CF1-A243-8D0E-1312D096DE88}">
+  <dimension ref="A2:F38"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="17">
+        <v>53436</v>
+      </c>
+      <c r="C3" s="17">
+        <v>56424</v>
+      </c>
+      <c r="D3" s="17">
+        <v>59948</v>
+      </c>
+      <c r="E3" s="17">
+        <v>59474</v>
+      </c>
+      <c r="F3" s="17">
+        <v>59788</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1707</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1803</v>
+      </c>
+      <c r="D4" s="17">
+        <v>2172</v>
+      </c>
+      <c r="E4" s="17">
+        <v>2117</v>
+      </c>
+      <c r="F4" s="17">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="17">
+        <v>4263</v>
+      </c>
+      <c r="C5" s="17">
+        <v>4244</v>
+      </c>
+      <c r="D5" s="17">
+        <v>4579</v>
+      </c>
+      <c r="E5" s="17">
+        <v>4539</v>
+      </c>
+      <c r="F5" s="17">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="17">
+        <v>5248</v>
+      </c>
+      <c r="C6" s="17">
+        <v>5224</v>
+      </c>
+      <c r="D6" s="17">
+        <v>5449</v>
+      </c>
+      <c r="E6" s="17">
+        <v>5497</v>
+      </c>
+      <c r="F6" s="17">
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="17">
+        <v>2104</v>
+      </c>
+      <c r="C7" s="17">
+        <v>2344</v>
+      </c>
+      <c r="D7" s="17">
+        <v>2382</v>
+      </c>
+      <c r="E7" s="17">
+        <v>2326</v>
+      </c>
+      <c r="F7" s="17">
+        <v>2369</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="17">
+        <v>13697</v>
+      </c>
+      <c r="C8" s="17">
+        <v>12899</v>
+      </c>
+      <c r="D8" s="17">
+        <v>11073</v>
+      </c>
+      <c r="E8" s="17">
+        <v>10710</v>
+      </c>
+      <c r="F8" s="17">
+        <v>10360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="17">
+        <v>17225</v>
+      </c>
+      <c r="C9" s="17">
+        <v>18786</v>
+      </c>
+      <c r="D9" s="17">
+        <v>20886</v>
+      </c>
+      <c r="E9" s="17">
+        <v>20831</v>
+      </c>
+      <c r="F9" s="17">
+        <v>21074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="17">
+        <v>2879</v>
+      </c>
+      <c r="C10" s="17">
+        <v>3792</v>
+      </c>
+      <c r="D10" s="17">
+        <v>4528</v>
+      </c>
+      <c r="E10" s="17">
+        <v>4687</v>
+      </c>
+      <c r="F10" s="17">
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="17">
+        <v>3008</v>
+      </c>
+      <c r="C11" s="17">
+        <v>3045</v>
+      </c>
+      <c r="D11" s="17">
+        <v>3707</v>
+      </c>
+      <c r="E11" s="17">
+        <v>3615</v>
+      </c>
+      <c r="F11" s="17">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="17">
+        <v>3305</v>
+      </c>
+      <c r="C12" s="17">
+        <v>4287</v>
+      </c>
+      <c r="D12" s="17">
+        <v>5172</v>
+      </c>
+      <c r="E12" s="17">
+        <v>5152</v>
+      </c>
+      <c r="F12" s="17">
+        <v>5171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="17">
+        <v>92985</v>
+      </c>
+      <c r="C13" s="17">
+        <v>77985</v>
+      </c>
+      <c r="D13" s="17">
+        <v>86534</v>
+      </c>
+      <c r="E13" s="17">
+        <v>86774</v>
+      </c>
+      <c r="F13" s="17">
+        <v>92311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="17">
+        <v>5867</v>
+      </c>
+      <c r="C14" s="17">
+        <v>8119</v>
+      </c>
+      <c r="D14" s="17">
+        <v>11817</v>
+      </c>
+      <c r="E14" s="17">
+        <v>12156</v>
+      </c>
+      <c r="F14" s="17">
+        <v>13636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="17">
+        <v>53593</v>
+      </c>
+      <c r="C15" s="17">
+        <v>39133</v>
+      </c>
+      <c r="D15" s="17">
+        <v>37099</v>
+      </c>
+      <c r="E15" s="17">
+        <v>36197</v>
+      </c>
+      <c r="F15" s="17">
+        <v>38777</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="17">
+        <v>15424</v>
+      </c>
+      <c r="C16" s="17">
+        <v>17182</v>
+      </c>
+      <c r="D16" s="17">
+        <v>21287</v>
+      </c>
+      <c r="E16" s="17">
+        <v>21709</v>
+      </c>
+      <c r="F16" s="17">
+        <v>22112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="17">
+        <v>18101</v>
+      </c>
+      <c r="C17" s="17">
+        <v>13551</v>
+      </c>
+      <c r="D17" s="17">
+        <v>16331</v>
+      </c>
+      <c r="E17" s="17">
+        <v>16712</v>
+      </c>
+      <c r="F17" s="17">
+        <v>17786</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="17">
+        <v>10884</v>
+      </c>
+      <c r="C18" s="17">
+        <v>8167</v>
+      </c>
+      <c r="D18" s="17">
+        <v>8500</v>
+      </c>
+      <c r="E18" s="17">
+        <v>7096</v>
+      </c>
+      <c r="F18" s="17">
+        <v>38339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="17">
+        <v>133</v>
+      </c>
+      <c r="C19" s="17">
+        <v>75</v>
+      </c>
+      <c r="D19" s="17">
+        <v>79</v>
+      </c>
+      <c r="E19" s="17">
+        <v>67</v>
+      </c>
+      <c r="F19" s="17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="17">
+        <v>10616</v>
+      </c>
+      <c r="C20" s="17">
+        <v>7977</v>
+      </c>
+      <c r="D20" s="17">
+        <v>8318</v>
+      </c>
+      <c r="E20" s="17">
+        <v>6914</v>
+      </c>
+      <c r="F20" s="17">
+        <v>38165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="17">
+        <v>135</v>
+      </c>
+      <c r="C21" s="17">
+        <v>115</v>
+      </c>
+      <c r="D21" s="17">
+        <v>103</v>
+      </c>
+      <c r="E21" s="17">
+        <v>115</v>
+      </c>
+      <c r="F21" s="17">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="17">
+        <v>14758</v>
+      </c>
+      <c r="C22" s="17">
+        <v>16088</v>
+      </c>
+      <c r="D22" s="17">
+        <v>20933</v>
+      </c>
+      <c r="E22" s="17">
+        <v>21628</v>
+      </c>
+      <c r="F22" s="17">
+        <v>24254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="17">
+        <v>2151</v>
+      </c>
+      <c r="C23" s="17">
+        <v>1961</v>
+      </c>
+      <c r="D23" s="17">
+        <v>1967</v>
+      </c>
+      <c r="E23" s="17">
+        <v>1849</v>
+      </c>
+      <c r="F23" s="17">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="17">
+        <v>5421</v>
+      </c>
+      <c r="C24" s="17">
+        <v>7336</v>
+      </c>
+      <c r="D24" s="17">
+        <v>10324</v>
+      </c>
+      <c r="E24" s="17">
+        <v>11332</v>
+      </c>
+      <c r="F24" s="17">
+        <v>13402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="17">
+        <v>4073</v>
+      </c>
+      <c r="C25" s="17">
+        <v>2986</v>
+      </c>
+      <c r="D25" s="17">
+        <v>4219</v>
+      </c>
+      <c r="E25" s="17">
+        <v>4104</v>
+      </c>
+      <c r="F25" s="17">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="17">
+        <v>3113</v>
+      </c>
+      <c r="C26" s="17">
+        <v>3805</v>
+      </c>
+      <c r="D26" s="17">
+        <v>4423</v>
+      </c>
+      <c r="E26" s="17">
+        <v>4343</v>
+      </c>
+      <c r="F26" s="17">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="17">
+        <v>14640</v>
+      </c>
+      <c r="C27" s="17">
+        <v>17519</v>
+      </c>
+      <c r="D27" s="17">
+        <v>22706</v>
+      </c>
+      <c r="E27" s="17">
+        <v>23544</v>
+      </c>
+      <c r="F27" s="17">
+        <v>26635</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="17">
+        <v>2127</v>
+      </c>
+      <c r="C28" s="17">
+        <v>3871</v>
+      </c>
+      <c r="D28" s="17">
+        <v>7545</v>
+      </c>
+      <c r="E28" s="17">
+        <v>7777</v>
+      </c>
+      <c r="F28" s="17">
+        <v>8707</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="17">
+        <v>3319</v>
+      </c>
+      <c r="C29" s="17">
+        <v>4468</v>
+      </c>
+      <c r="D29" s="17">
+        <v>4845</v>
+      </c>
+      <c r="E29" s="17">
+        <v>5259</v>
+      </c>
+      <c r="F29" s="17">
+        <v>7636</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="17">
+        <v>4579</v>
+      </c>
+      <c r="C30" s="17">
+        <v>4209</v>
+      </c>
+      <c r="D30" s="17">
+        <v>4504</v>
+      </c>
+      <c r="E30" s="17">
+        <v>4673</v>
+      </c>
+      <c r="F30" s="17">
+        <v>4815</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="17">
+        <v>2984</v>
+      </c>
+      <c r="C31" s="17">
+        <v>3506</v>
+      </c>
+      <c r="D31" s="17">
+        <v>4630</v>
+      </c>
+      <c r="E31" s="17">
+        <v>4715</v>
+      </c>
+      <c r="F31" s="17">
+        <v>4502</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="17">
+        <v>1631</v>
+      </c>
+      <c r="C32" s="17">
+        <v>1465</v>
+      </c>
+      <c r="D32" s="17">
+        <v>1182</v>
+      </c>
+      <c r="E32" s="17">
+        <v>1120</v>
+      </c>
+      <c r="F32" s="17">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="17">
+        <v>41578</v>
+      </c>
+      <c r="C33" s="17">
+        <v>55478</v>
+      </c>
+      <c r="D33" s="17">
+        <v>67539</v>
+      </c>
+      <c r="E33" s="17">
+        <v>68515</v>
+      </c>
+      <c r="F33" s="17">
+        <v>75213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="17">
+        <v>6000</v>
+      </c>
+      <c r="C34" s="17">
+        <v>6332</v>
+      </c>
+      <c r="D34" s="17">
+        <v>5936</v>
+      </c>
+      <c r="E34" s="17">
+        <v>6151</v>
+      </c>
+      <c r="F34" s="17">
+        <v>7407</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="17">
+        <v>4154</v>
+      </c>
+      <c r="C35" s="17">
+        <v>5027</v>
+      </c>
+      <c r="D35" s="17">
+        <v>6204</v>
+      </c>
+      <c r="E35" s="17">
+        <v>6377</v>
+      </c>
+      <c r="F35" s="17">
+        <v>7035</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="17">
+        <v>10444</v>
+      </c>
+      <c r="C36" s="17">
+        <v>22719</v>
+      </c>
+      <c r="D36" s="17">
+        <v>31802</v>
+      </c>
+      <c r="E36" s="17">
+        <v>32937</v>
+      </c>
+      <c r="F36" s="17">
+        <v>36843</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="17">
+        <v>20980</v>
+      </c>
+      <c r="C37" s="17">
+        <v>21400</v>
+      </c>
+      <c r="D37" s="17">
+        <v>23597</v>
+      </c>
+      <c r="E37" s="17">
+        <v>23050</v>
+      </c>
+      <c r="F37" s="17">
+        <v>23928</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" s="17">
+        <v>228281</v>
+      </c>
+      <c r="C38" s="17">
+        <v>231661</v>
+      </c>
+      <c r="D38" s="17">
+        <v>266160</v>
+      </c>
+      <c r="E38" s="17">
+        <v>267031</v>
+      </c>
+      <c r="F38" s="17">
+        <v>316540</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401F6810-FA8E-7647-9C40-841F9AFF83D4}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="8">
+        <v>54333</v>
+      </c>
+      <c r="C3" s="8">
+        <v>53436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="9">
+        <v>92982</v>
+      </c>
+      <c r="C4" s="9">
+        <v>92985</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="9">
+        <v>4700</v>
+      </c>
+      <c r="C5" s="9">
+        <v>10884</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="9">
+        <v>14002</v>
+      </c>
+      <c r="C6" s="9">
+        <v>14758</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="9">
+        <v>31791</v>
+      </c>
+      <c r="C7" s="9">
+        <v>14640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="9">
+        <v>31889</v>
+      </c>
+      <c r="C8" s="9">
+        <v>41578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="8">
+        <f>SUM(B3:B8)</f>
+        <v>229697</v>
+      </c>
+      <c r="C9" s="8">
+        <f>SUM(C3:C8)</f>
+        <v>228281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
+        <v>2010</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="14">
+        <v>57820</v>
+      </c>
+      <c r="C13" s="14">
+        <v>56424</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="11">
+        <v>78960</v>
+      </c>
+      <c r="C14" s="11">
+        <v>77985</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="11">
+        <v>6147</v>
+      </c>
+      <c r="C15" s="11">
+        <v>8167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="11">
+        <v>16855</v>
+      </c>
+      <c r="C16" s="11">
+        <v>16088</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="11">
+        <v>33808</v>
+      </c>
+      <c r="C17" s="11">
+        <v>17519</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="11">
+        <v>41250</v>
+      </c>
+      <c r="C18" s="11">
+        <v>55478</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="14">
+        <f>SUM(B13:B18)</f>
+        <v>234840</v>
+      </c>
+      <c r="C19" s="14">
+        <f>SUM(C13:C18)</f>
+        <v>231661</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
+        <v>2018</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="14">
+        <v>61300</v>
+      </c>
+      <c r="C23" s="14">
+        <v>59948</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="11">
+        <v>87282</v>
+      </c>
+      <c r="C24" s="11">
+        <v>86534</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="11">
+        <v>6785</v>
+      </c>
+      <c r="C25" s="11">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="11">
+        <v>21159</v>
+      </c>
+      <c r="C26" s="11">
+        <v>20933</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="11">
+        <v>41338</v>
+      </c>
+      <c r="C27" s="11">
+        <v>22706</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="11">
+        <v>51553</v>
+      </c>
+      <c r="C28" s="11">
+        <v>67539</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="14">
+        <f>SUM(B23:B28)</f>
+        <v>269417</v>
+      </c>
+      <c r="C29" s="14">
+        <f>SUM(C23:C28)</f>
+        <v>266160</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A21:C21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed "total from cdc" and "total from ccb" rows from the "ccb_cause_to_100_year_cause" tab of the "ccb_cause_to_100_year_cause" document.
</commit_message>
<xml_diff>
--- a/ccb_cause_to_100_year_cause.xlsx
+++ b/ccb_cause_to_100_year_cause.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B536998-8209-8E4B-9569-CBCB569CEFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB744863-B095-494D-B7C0-8C2744B4959A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ccb_cause_to_100_year_causes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="147" r:id="rId4"/>
+    <pivotCache cacheId="149" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="166">
   <si>
     <t>causeCode</t>
   </si>
@@ -507,12 +507,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Total from ccb data</t>
-  </si>
-  <si>
-    <t>Total from cdc data</t>
   </si>
   <si>
     <t>CDC WONDER</t>
@@ -636,15 +630,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -655,9 +644,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -665,6 +651,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,7 +1356,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="147" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="149" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:F38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1852,11 +1844,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3750,55 +3742,6 @@
       <c r="E60" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3">
-        <f>SUM(F2:F60)</f>
-        <v>228281</v>
-      </c>
-      <c r="G61" s="3">
-        <f t="shared" ref="G61:J61" si="0">SUM(G2:G60)</f>
-        <v>231661</v>
-      </c>
-      <c r="H61" s="3">
-        <f t="shared" si="0"/>
-        <v>266160</v>
-      </c>
-      <c r="I61" s="3">
-        <f t="shared" si="0"/>
-        <v>267031</v>
-      </c>
-      <c r="J61" s="3">
-        <f t="shared" si="0"/>
-        <v>316540</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1">
-        <v>229697</v>
-      </c>
-      <c r="G62" s="1">
-        <v>234840</v>
-      </c>
-      <c r="H62" s="1">
-        <v>269417</v>
-      </c>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
@@ -3826,742 +3769,742 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
         <v>162</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="13">
+        <v>53436</v>
+      </c>
+      <c r="C3" s="13">
+        <v>56424</v>
+      </c>
+      <c r="D3" s="13">
+        <v>59948</v>
+      </c>
+      <c r="E3" s="13">
+        <v>59474</v>
+      </c>
+      <c r="F3" s="13">
+        <v>59788</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1707</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1803</v>
+      </c>
+      <c r="D4" s="13">
+        <v>2172</v>
+      </c>
+      <c r="E4" s="13">
+        <v>2117</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="13">
+        <v>4263</v>
+      </c>
+      <c r="C5" s="13">
+        <v>4244</v>
+      </c>
+      <c r="D5" s="13">
+        <v>4579</v>
+      </c>
+      <c r="E5" s="13">
+        <v>4539</v>
+      </c>
+      <c r="F5" s="13">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="13">
+        <v>5248</v>
+      </c>
+      <c r="C6" s="13">
+        <v>5224</v>
+      </c>
+      <c r="D6" s="13">
+        <v>5449</v>
+      </c>
+      <c r="E6" s="13">
+        <v>5497</v>
+      </c>
+      <c r="F6" s="13">
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="13">
+        <v>2104</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2344</v>
+      </c>
+      <c r="D7" s="13">
+        <v>2382</v>
+      </c>
+      <c r="E7" s="13">
+        <v>2326</v>
+      </c>
+      <c r="F7" s="13">
+        <v>2369</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="13">
+        <v>13697</v>
+      </c>
+      <c r="C8" s="13">
+        <v>12899</v>
+      </c>
+      <c r="D8" s="13">
+        <v>11073</v>
+      </c>
+      <c r="E8" s="13">
+        <v>10710</v>
+      </c>
+      <c r="F8" s="13">
+        <v>10360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="13">
+        <v>17225</v>
+      </c>
+      <c r="C9" s="13">
+        <v>18786</v>
+      </c>
+      <c r="D9" s="13">
+        <v>20886</v>
+      </c>
+      <c r="E9" s="13">
+        <v>20831</v>
+      </c>
+      <c r="F9" s="13">
+        <v>21074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="13">
+        <v>2879</v>
+      </c>
+      <c r="C10" s="13">
+        <v>3792</v>
+      </c>
+      <c r="D10" s="13">
+        <v>4528</v>
+      </c>
+      <c r="E10" s="13">
+        <v>4687</v>
+      </c>
+      <c r="F10" s="13">
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="13">
+        <v>3008</v>
+      </c>
+      <c r="C11" s="13">
+        <v>3045</v>
+      </c>
+      <c r="D11" s="13">
+        <v>3707</v>
+      </c>
+      <c r="E11" s="13">
+        <v>3615</v>
+      </c>
+      <c r="F11" s="13">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="13">
+        <v>3305</v>
+      </c>
+      <c r="C12" s="13">
+        <v>4287</v>
+      </c>
+      <c r="D12" s="13">
+        <v>5172</v>
+      </c>
+      <c r="E12" s="13">
+        <v>5152</v>
+      </c>
+      <c r="F12" s="13">
+        <v>5171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="13">
+        <v>92985</v>
+      </c>
+      <c r="C13" s="13">
+        <v>77985</v>
+      </c>
+      <c r="D13" s="13">
+        <v>86534</v>
+      </c>
+      <c r="E13" s="13">
+        <v>86774</v>
+      </c>
+      <c r="F13" s="13">
+        <v>92311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="13">
+        <v>5867</v>
+      </c>
+      <c r="C14" s="13">
+        <v>8119</v>
+      </c>
+      <c r="D14" s="13">
+        <v>11817</v>
+      </c>
+      <c r="E14" s="13">
+        <v>12156</v>
+      </c>
+      <c r="F14" s="13">
+        <v>13636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="13">
+        <v>53593</v>
+      </c>
+      <c r="C15" s="13">
+        <v>39133</v>
+      </c>
+      <c r="D15" s="13">
+        <v>37099</v>
+      </c>
+      <c r="E15" s="13">
+        <v>36197</v>
+      </c>
+      <c r="F15" s="13">
+        <v>38777</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="13">
+        <v>15424</v>
+      </c>
+      <c r="C16" s="13">
+        <v>17182</v>
+      </c>
+      <c r="D16" s="13">
+        <v>21287</v>
+      </c>
+      <c r="E16" s="13">
+        <v>21709</v>
+      </c>
+      <c r="F16" s="13">
+        <v>22112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="13">
+        <v>18101</v>
+      </c>
+      <c r="C17" s="13">
+        <v>13551</v>
+      </c>
+      <c r="D17" s="13">
+        <v>16331</v>
+      </c>
+      <c r="E17" s="13">
+        <v>16712</v>
+      </c>
+      <c r="F17" s="13">
+        <v>17786</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="13">
+        <v>10884</v>
+      </c>
+      <c r="C18" s="13">
+        <v>8167</v>
+      </c>
+      <c r="D18" s="13">
+        <v>8500</v>
+      </c>
+      <c r="E18" s="13">
+        <v>7096</v>
+      </c>
+      <c r="F18" s="13">
+        <v>38339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="13">
+        <v>133</v>
+      </c>
+      <c r="C19" s="13">
+        <v>75</v>
+      </c>
+      <c r="D19" s="13">
+        <v>79</v>
+      </c>
+      <c r="E19" s="13">
+        <v>67</v>
+      </c>
+      <c r="F19" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="13">
+        <v>10616</v>
+      </c>
+      <c r="C20" s="13">
+        <v>7977</v>
+      </c>
+      <c r="D20" s="13">
+        <v>8318</v>
+      </c>
+      <c r="E20" s="13">
+        <v>6914</v>
+      </c>
+      <c r="F20" s="13">
+        <v>38165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="13">
+        <v>135</v>
+      </c>
+      <c r="C21" s="13">
+        <v>115</v>
+      </c>
+      <c r="D21" s="13">
+        <v>103</v>
+      </c>
+      <c r="E21" s="13">
+        <v>115</v>
+      </c>
+      <c r="F21" s="13">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="13">
+        <v>14758</v>
+      </c>
+      <c r="C22" s="13">
+        <v>16088</v>
+      </c>
+      <c r="D22" s="13">
+        <v>20933</v>
+      </c>
+      <c r="E22" s="13">
+        <v>21628</v>
+      </c>
+      <c r="F22" s="13">
+        <v>24254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="13">
+        <v>2151</v>
+      </c>
+      <c r="C23" s="13">
+        <v>1961</v>
+      </c>
+      <c r="D23" s="13">
+        <v>1967</v>
+      </c>
+      <c r="E23" s="13">
+        <v>1849</v>
+      </c>
+      <c r="F23" s="13">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="13">
+        <v>5421</v>
+      </c>
+      <c r="C24" s="13">
+        <v>7336</v>
+      </c>
+      <c r="D24" s="13">
+        <v>10324</v>
+      </c>
+      <c r="E24" s="13">
+        <v>11332</v>
+      </c>
+      <c r="F24" s="13">
+        <v>13402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="13">
+        <v>4073</v>
+      </c>
+      <c r="C25" s="13">
+        <v>2986</v>
+      </c>
+      <c r="D25" s="13">
+        <v>4219</v>
+      </c>
+      <c r="E25" s="13">
+        <v>4104</v>
+      </c>
+      <c r="F25" s="13">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="13">
+        <v>3113</v>
+      </c>
+      <c r="C26" s="13">
+        <v>3805</v>
+      </c>
+      <c r="D26" s="13">
+        <v>4423</v>
+      </c>
+      <c r="E26" s="13">
+        <v>4343</v>
+      </c>
+      <c r="F26" s="13">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="13">
+        <v>14640</v>
+      </c>
+      <c r="C27" s="13">
+        <v>17519</v>
+      </c>
+      <c r="D27" s="13">
+        <v>22706</v>
+      </c>
+      <c r="E27" s="13">
+        <v>23544</v>
+      </c>
+      <c r="F27" s="13">
+        <v>26635</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="13">
+        <v>2127</v>
+      </c>
+      <c r="C28" s="13">
+        <v>3871</v>
+      </c>
+      <c r="D28" s="13">
+        <v>7545</v>
+      </c>
+      <c r="E28" s="13">
+        <v>7777</v>
+      </c>
+      <c r="F28" s="13">
+        <v>8707</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="13">
+        <v>3319</v>
+      </c>
+      <c r="C29" s="13">
+        <v>4468</v>
+      </c>
+      <c r="D29" s="13">
+        <v>4845</v>
+      </c>
+      <c r="E29" s="13">
+        <v>5259</v>
+      </c>
+      <c r="F29" s="13">
+        <v>7636</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="13">
+        <v>4579</v>
+      </c>
+      <c r="C30" s="13">
+        <v>4209</v>
+      </c>
+      <c r="D30" s="13">
+        <v>4504</v>
+      </c>
+      <c r="E30" s="13">
+        <v>4673</v>
+      </c>
+      <c r="F30" s="13">
+        <v>4815</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="13">
+        <v>2984</v>
+      </c>
+      <c r="C31" s="13">
+        <v>3506</v>
+      </c>
+      <c r="D31" s="13">
+        <v>4630</v>
+      </c>
+      <c r="E31" s="13">
+        <v>4715</v>
+      </c>
+      <c r="F31" s="13">
+        <v>4502</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="13">
+        <v>1631</v>
+      </c>
+      <c r="C32" s="13">
+        <v>1465</v>
+      </c>
+      <c r="D32" s="13">
+        <v>1182</v>
+      </c>
+      <c r="E32" s="13">
+        <v>1120</v>
+      </c>
+      <c r="F32" s="13">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="13">
+        <v>41578</v>
+      </c>
+      <c r="C33" s="13">
+        <v>55478</v>
+      </c>
+      <c r="D33" s="13">
+        <v>67539</v>
+      </c>
+      <c r="E33" s="13">
+        <v>68515</v>
+      </c>
+      <c r="F33" s="13">
+        <v>75213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="13">
+        <v>6000</v>
+      </c>
+      <c r="C34" s="13">
+        <v>6332</v>
+      </c>
+      <c r="D34" s="13">
+        <v>5936</v>
+      </c>
+      <c r="E34" s="13">
+        <v>6151</v>
+      </c>
+      <c r="F34" s="13">
+        <v>7407</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="13">
+        <v>4154</v>
+      </c>
+      <c r="C35" s="13">
+        <v>5027</v>
+      </c>
+      <c r="D35" s="13">
+        <v>6204</v>
+      </c>
+      <c r="E35" s="13">
+        <v>6377</v>
+      </c>
+      <c r="F35" s="13">
+        <v>7035</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="13">
+        <v>10444</v>
+      </c>
+      <c r="C36" s="13">
+        <v>22719</v>
+      </c>
+      <c r="D36" s="13">
+        <v>31802</v>
+      </c>
+      <c r="E36" s="13">
+        <v>32937</v>
+      </c>
+      <c r="F36" s="13">
+        <v>36843</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="13">
+        <v>20980</v>
+      </c>
+      <c r="C37" s="13">
+        <v>21400</v>
+      </c>
+      <c r="D37" s="13">
+        <v>23597</v>
+      </c>
+      <c r="E37" s="13">
+        <v>23050</v>
+      </c>
+      <c r="F37" s="13">
+        <v>23928</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="C2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="17">
-        <v>53436</v>
-      </c>
-      <c r="C3" s="17">
-        <v>56424</v>
-      </c>
-      <c r="D3" s="17">
-        <v>59948</v>
-      </c>
-      <c r="E3" s="17">
-        <v>59474</v>
-      </c>
-      <c r="F3" s="17">
-        <v>59788</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="17">
-        <v>1707</v>
-      </c>
-      <c r="C4" s="17">
-        <v>1803</v>
-      </c>
-      <c r="D4" s="17">
-        <v>2172</v>
-      </c>
-      <c r="E4" s="17">
-        <v>2117</v>
-      </c>
-      <c r="F4" s="17">
-        <v>2306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="17">
-        <v>4263</v>
-      </c>
-      <c r="C5" s="17">
-        <v>4244</v>
-      </c>
-      <c r="D5" s="17">
-        <v>4579</v>
-      </c>
-      <c r="E5" s="17">
-        <v>4539</v>
-      </c>
-      <c r="F5" s="17">
-        <v>4540</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="17">
-        <v>5248</v>
-      </c>
-      <c r="C6" s="17">
-        <v>5224</v>
-      </c>
-      <c r="D6" s="17">
-        <v>5449</v>
-      </c>
-      <c r="E6" s="17">
-        <v>5497</v>
-      </c>
-      <c r="F6" s="17">
-        <v>5520</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="17">
-        <v>2104</v>
-      </c>
-      <c r="C7" s="17">
-        <v>2344</v>
-      </c>
-      <c r="D7" s="17">
-        <v>2382</v>
-      </c>
-      <c r="E7" s="17">
-        <v>2326</v>
-      </c>
-      <c r="F7" s="17">
-        <v>2369</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="17">
-        <v>13697</v>
-      </c>
-      <c r="C8" s="17">
-        <v>12899</v>
-      </c>
-      <c r="D8" s="17">
-        <v>11073</v>
-      </c>
-      <c r="E8" s="17">
-        <v>10710</v>
-      </c>
-      <c r="F8" s="17">
-        <v>10360</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="17">
-        <v>17225</v>
-      </c>
-      <c r="C9" s="17">
-        <v>18786</v>
-      </c>
-      <c r="D9" s="17">
-        <v>20886</v>
-      </c>
-      <c r="E9" s="17">
-        <v>20831</v>
-      </c>
-      <c r="F9" s="17">
-        <v>21074</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="17">
-        <v>2879</v>
-      </c>
-      <c r="C10" s="17">
-        <v>3792</v>
-      </c>
-      <c r="D10" s="17">
-        <v>4528</v>
-      </c>
-      <c r="E10" s="17">
-        <v>4687</v>
-      </c>
-      <c r="F10" s="17">
-        <v>4637</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="17">
-        <v>3008</v>
-      </c>
-      <c r="C11" s="17">
-        <v>3045</v>
-      </c>
-      <c r="D11" s="17">
-        <v>3707</v>
-      </c>
-      <c r="E11" s="17">
-        <v>3615</v>
-      </c>
-      <c r="F11" s="17">
-        <v>3811</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="17">
-        <v>3305</v>
-      </c>
-      <c r="C12" s="17">
-        <v>4287</v>
-      </c>
-      <c r="D12" s="17">
-        <v>5172</v>
-      </c>
-      <c r="E12" s="17">
-        <v>5152</v>
-      </c>
-      <c r="F12" s="17">
-        <v>5171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="17">
-        <v>92985</v>
-      </c>
-      <c r="C13" s="17">
-        <v>77985</v>
-      </c>
-      <c r="D13" s="17">
-        <v>86534</v>
-      </c>
-      <c r="E13" s="17">
-        <v>86774</v>
-      </c>
-      <c r="F13" s="17">
-        <v>92311</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="17">
-        <v>5867</v>
-      </c>
-      <c r="C14" s="17">
-        <v>8119</v>
-      </c>
-      <c r="D14" s="17">
-        <v>11817</v>
-      </c>
-      <c r="E14" s="17">
-        <v>12156</v>
-      </c>
-      <c r="F14" s="17">
-        <v>13636</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="17">
-        <v>53593</v>
-      </c>
-      <c r="C15" s="17">
-        <v>39133</v>
-      </c>
-      <c r="D15" s="17">
-        <v>37099</v>
-      </c>
-      <c r="E15" s="17">
-        <v>36197</v>
-      </c>
-      <c r="F15" s="17">
-        <v>38777</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="17">
-        <v>15424</v>
-      </c>
-      <c r="C16" s="17">
-        <v>17182</v>
-      </c>
-      <c r="D16" s="17">
-        <v>21287</v>
-      </c>
-      <c r="E16" s="17">
-        <v>21709</v>
-      </c>
-      <c r="F16" s="17">
-        <v>22112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="17">
-        <v>18101</v>
-      </c>
-      <c r="C17" s="17">
-        <v>13551</v>
-      </c>
-      <c r="D17" s="17">
-        <v>16331</v>
-      </c>
-      <c r="E17" s="17">
-        <v>16712</v>
-      </c>
-      <c r="F17" s="17">
-        <v>17786</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="17">
-        <v>10884</v>
-      </c>
-      <c r="C18" s="17">
-        <v>8167</v>
-      </c>
-      <c r="D18" s="17">
-        <v>8500</v>
-      </c>
-      <c r="E18" s="17">
-        <v>7096</v>
-      </c>
-      <c r="F18" s="17">
-        <v>38339</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="17">
-        <v>133</v>
-      </c>
-      <c r="C19" s="17">
-        <v>75</v>
-      </c>
-      <c r="D19" s="17">
-        <v>79</v>
-      </c>
-      <c r="E19" s="17">
-        <v>67</v>
-      </c>
-      <c r="F19" s="17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="17">
-        <v>10616</v>
-      </c>
-      <c r="C20" s="17">
-        <v>7977</v>
-      </c>
-      <c r="D20" s="17">
-        <v>8318</v>
-      </c>
-      <c r="E20" s="17">
-        <v>6914</v>
-      </c>
-      <c r="F20" s="17">
-        <v>38165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="17">
-        <v>135</v>
-      </c>
-      <c r="C21" s="17">
-        <v>115</v>
-      </c>
-      <c r="D21" s="17">
-        <v>103</v>
-      </c>
-      <c r="E21" s="17">
-        <v>115</v>
-      </c>
-      <c r="F21" s="17">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B22" s="17">
-        <v>14758</v>
-      </c>
-      <c r="C22" s="17">
-        <v>16088</v>
-      </c>
-      <c r="D22" s="17">
-        <v>20933</v>
-      </c>
-      <c r="E22" s="17">
-        <v>21628</v>
-      </c>
-      <c r="F22" s="17">
-        <v>24254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="17">
-        <v>2151</v>
-      </c>
-      <c r="C23" s="17">
-        <v>1961</v>
-      </c>
-      <c r="D23" s="17">
-        <v>1967</v>
-      </c>
-      <c r="E23" s="17">
-        <v>1849</v>
-      </c>
-      <c r="F23" s="17">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="17">
-        <v>5421</v>
-      </c>
-      <c r="C24" s="17">
-        <v>7336</v>
-      </c>
-      <c r="D24" s="17">
-        <v>10324</v>
-      </c>
-      <c r="E24" s="17">
-        <v>11332</v>
-      </c>
-      <c r="F24" s="17">
-        <v>13402</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" s="17">
-        <v>4073</v>
-      </c>
-      <c r="C25" s="17">
-        <v>2986</v>
-      </c>
-      <c r="D25" s="17">
-        <v>4219</v>
-      </c>
-      <c r="E25" s="17">
-        <v>4104</v>
-      </c>
-      <c r="F25" s="17">
-        <v>4468</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B26" s="17">
-        <v>3113</v>
-      </c>
-      <c r="C26" s="17">
-        <v>3805</v>
-      </c>
-      <c r="D26" s="17">
-        <v>4423</v>
-      </c>
-      <c r="E26" s="17">
-        <v>4343</v>
-      </c>
-      <c r="F26" s="17">
-        <v>3992</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="17">
-        <v>14640</v>
-      </c>
-      <c r="C27" s="17">
-        <v>17519</v>
-      </c>
-      <c r="D27" s="17">
-        <v>22706</v>
-      </c>
-      <c r="E27" s="17">
-        <v>23544</v>
-      </c>
-      <c r="F27" s="17">
-        <v>26635</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="17">
-        <v>2127</v>
-      </c>
-      <c r="C28" s="17">
-        <v>3871</v>
-      </c>
-      <c r="D28" s="17">
-        <v>7545</v>
-      </c>
-      <c r="E28" s="17">
-        <v>7777</v>
-      </c>
-      <c r="F28" s="17">
-        <v>8707</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="17">
-        <v>3319</v>
-      </c>
-      <c r="C29" s="17">
-        <v>4468</v>
-      </c>
-      <c r="D29" s="17">
-        <v>4845</v>
-      </c>
-      <c r="E29" s="17">
-        <v>5259</v>
-      </c>
-      <c r="F29" s="17">
-        <v>7636</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="17">
-        <v>4579</v>
-      </c>
-      <c r="C30" s="17">
-        <v>4209</v>
-      </c>
-      <c r="D30" s="17">
-        <v>4504</v>
-      </c>
-      <c r="E30" s="17">
-        <v>4673</v>
-      </c>
-      <c r="F30" s="17">
-        <v>4815</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="B31" s="17">
-        <v>2984</v>
-      </c>
-      <c r="C31" s="17">
-        <v>3506</v>
-      </c>
-      <c r="D31" s="17">
-        <v>4630</v>
-      </c>
-      <c r="E31" s="17">
-        <v>4715</v>
-      </c>
-      <c r="F31" s="17">
-        <v>4502</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="17">
-        <v>1631</v>
-      </c>
-      <c r="C32" s="17">
-        <v>1465</v>
-      </c>
-      <c r="D32" s="17">
-        <v>1182</v>
-      </c>
-      <c r="E32" s="17">
-        <v>1120</v>
-      </c>
-      <c r="F32" s="17">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" s="17">
-        <v>41578</v>
-      </c>
-      <c r="C33" s="17">
-        <v>55478</v>
-      </c>
-      <c r="D33" s="17">
-        <v>67539</v>
-      </c>
-      <c r="E33" s="17">
-        <v>68515</v>
-      </c>
-      <c r="F33" s="17">
-        <v>75213</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="17">
-        <v>6000</v>
-      </c>
-      <c r="C34" s="17">
-        <v>6332</v>
-      </c>
-      <c r="D34" s="17">
-        <v>5936</v>
-      </c>
-      <c r="E34" s="17">
-        <v>6151</v>
-      </c>
-      <c r="F34" s="17">
-        <v>7407</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" s="17">
-        <v>4154</v>
-      </c>
-      <c r="C35" s="17">
-        <v>5027</v>
-      </c>
-      <c r="D35" s="17">
-        <v>6204</v>
-      </c>
-      <c r="E35" s="17">
-        <v>6377</v>
-      </c>
-      <c r="F35" s="17">
-        <v>7035</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="17">
-        <v>10444</v>
-      </c>
-      <c r="C36" s="17">
-        <v>22719</v>
-      </c>
-      <c r="D36" s="17">
-        <v>31802</v>
-      </c>
-      <c r="E36" s="17">
-        <v>32937</v>
-      </c>
-      <c r="F36" s="17">
-        <v>36843</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B37" s="17">
-        <v>20980</v>
-      </c>
-      <c r="C37" s="17">
-        <v>21400</v>
-      </c>
-      <c r="D37" s="17">
-        <v>23597</v>
-      </c>
-      <c r="E37" s="17">
-        <v>23050</v>
-      </c>
-      <c r="F37" s="17">
-        <v>23928</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="B38" s="17">
+      <c r="B38" s="13">
         <v>228281</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="13">
         <v>231661</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="13">
         <v>266160</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="13">
         <v>267031</v>
       </c>
-      <c r="F38" s="17">
+      <c r="F38" s="13">
         <v>316540</v>
       </c>
     </row>
@@ -4574,293 +4517,293 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401F6810-FA8E-7647-9C40-841F9AFF83D4}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+    <sheetView zoomScale="158" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5">
+      <c r="A1" s="17">
         <v>2000</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>160</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>54333</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="5">
         <v>53436</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>92982</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>92985</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>4700</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>10884</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>14002</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>14758</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>31791</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>14640</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="6">
         <v>31889</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="6">
         <v>41578</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="5">
         <f>SUM(B3:B8)</f>
         <v>229697</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="5">
         <f>SUM(C3:C8)</f>
         <v>228281</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+      <c r="A11" s="18">
         <v>2010</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>160</v>
+      <c r="A12" s="7"/>
+      <c r="B12" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>57820</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="11">
         <v>56424</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="8">
         <v>78960</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="8">
         <v>77985</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="8">
         <v>6147</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="8">
         <v>8167</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="8">
         <v>16855</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
         <v>16088</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="8">
         <v>33808</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <v>17519</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="8">
         <v>41250</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="8">
         <v>55478</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="11">
         <f>SUM(B13:B18)</f>
         <v>234840</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="11">
         <f>SUM(C13:C18)</f>
         <v>231661</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
+      <c r="A21" s="18">
         <v>2018</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>160</v>
+      <c r="A22" s="7"/>
+      <c r="B22" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="11">
         <v>61300</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="11">
         <v>59948</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="8">
         <v>87282</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="8">
         <v>86534</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="8">
         <v>6785</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="8">
         <v>8500</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="8">
         <v>21159</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="8">
         <v>20933</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="8">
         <v>41338</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="8">
         <v>22706</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="8">
         <v>51553</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="8">
         <v>67539</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="11">
         <f>SUM(B23:B28)</f>
         <v>269417</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="11">
         <f>SUM(C23:C28)</f>
         <v>266160</v>
       </c>

</xml_diff>

<commit_message>
OurGroup0, OurGroup1, and OurGroup3 were renamed to specificLevel, troubleshooting, and topLevel (respectively) in both of the excel spreadsheets as well as the R code. An additional category called "displayLevel" was added to the excel spreadsheets (13 categories not including COVID-19). All topLevel columns in excel were color coded and the troubleshooting categories were reviewed and reworked. Within the R code, plots for crude deathrates by topLevel and number of deaths by the troubleshooting category were added. All the plots were given descriptive titles with centered spacing, and some adjustments were made to x-axis horizontal alignment.
</commit_message>
<xml_diff>
--- a/ccb_cause_to_100_year_cause.xlsx
+++ b/ccb_cause_to_100_year_cause.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB744863-B095-494D-B7C0-8C2744B4959A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336DBAE2-B87F-3742-BF46-21116750C730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ccb_cause_to_100_year_causes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="149" r:id="rId4"/>
+    <pivotCache cacheId="150" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1356,7 +1356,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="149" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="150" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:F38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1846,9 +1846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4517,7 +4517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401F6810-FA8E-7647-9C40-841F9AFF83D4}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView zoomScale="158" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="158" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modified cardiovascular mortality comparison charts in the 1900-2020 excel file and made som adjustments to sortin of specificLevel and troubleshooting groups. Data from the CCB excel file was read into the R markdown file for the ccb years 2000, 2010, and 2018. A new block was created (the 4th block) that outputs comparison charts between CDC and CCB data in the form of a bar chart as well as a table (to do this, the formattable package was installed). The table compared 2000, 2010, and 2018 between ccb and cdc data broken down by specificLevel. The table was created in order to help understand and visualize the differences in sorting between the two mortality data sources. Additionally, a short statement describing the purpose of this project was added to the R markdown file.
</commit_message>
<xml_diff>
--- a/ccb_cause_to_100_year_cause.xlsx
+++ b/ccb_cause_to_100_year_cause.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336DBAE2-B87F-3742-BF46-21116750C730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C39E6D7-5BD8-4940-846D-D134374DD05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="150" r:id="rId4"/>
+    <pivotCache cacheId="188" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="167">
   <si>
     <t>causeCode</t>
   </si>
@@ -44,15 +44,6 @@
     <t>causeName</t>
   </si>
   <si>
-    <t>OurGroup0</t>
-  </si>
-  <si>
-    <t>OurGroup1</t>
-  </si>
-  <si>
-    <t>OurGroup3</t>
-  </si>
-  <si>
     <t>deaths_2000</t>
   </si>
   <si>
@@ -534,13 +525,25 @@
   </si>
   <si>
     <t>Sum of deaths_2019</t>
+  </si>
+  <si>
+    <t>specificLevel</t>
+  </si>
+  <si>
+    <t>troubleshooting</t>
+  </si>
+  <si>
+    <t>topLevel</t>
+  </si>
+  <si>
+    <t>displayLevel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -552,6 +555,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -630,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -652,6 +661,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,10 +674,73 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
     <dxf>
       <fill>
-        <patternFill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="gray0625">
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -686,7 +761,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="44385.688818750001" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="59" xr:uid="{1B34D8C8-DBA7-554E-AFCE-27F8C51D4782}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C1:J60" sheet="ccb_cause_to_100_year_causes"/>
+    <worksheetSource ref="C1:K60" sheet="ccb_cause_to_100_year_causes"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="OurGroup0" numFmtId="0">
@@ -1356,7 +1431,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="150" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="188" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:F38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1844,11 +1919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1856,10 +1931,11 @@
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="95.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1867,1886 +1943,2136 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="G2">
+        <v>135</v>
+      </c>
+      <c r="H2">
+        <v>115</v>
+      </c>
+      <c r="I2">
+        <v>103</v>
+      </c>
+      <c r="J2">
+        <v>115</v>
+      </c>
+      <c r="K2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="F2">
-        <v>135</v>
-      </c>
-      <c r="G2">
-        <v>115</v>
-      </c>
-      <c r="H2">
-        <v>103</v>
-      </c>
-      <c r="I2">
-        <v>115</v>
-      </c>
-      <c r="J2">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
         <v>1472</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>744</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>584</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>603</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>618</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
         <v>133</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>75</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>79</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>67</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5">
         <v>36</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>43</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>40</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>50</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6">
         <v>677</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1302</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>767</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>607</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>602</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
         <v>8431</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>5888</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>6927</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>5654</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>6042</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>59</v>
+      </c>
+      <c r="H8">
+        <v>80</v>
+      </c>
+      <c r="I8">
+        <v>86</v>
+      </c>
+      <c r="J8">
+        <v>68</v>
+      </c>
+      <c r="K8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>1572</v>
+      </c>
+      <c r="H9">
+        <v>1385</v>
+      </c>
+      <c r="I9">
+        <v>1096</v>
+      </c>
+      <c r="J9">
+        <v>1052</v>
+      </c>
+      <c r="K9">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="F8">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>30857</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>2150</v>
+      </c>
+      <c r="H11">
+        <v>3261</v>
+      </c>
+      <c r="I11">
+        <v>4127</v>
+      </c>
+      <c r="J11">
+        <v>4255</v>
+      </c>
+      <c r="K11">
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12">
+        <v>801</v>
+      </c>
+      <c r="H12">
+        <v>918</v>
+      </c>
+      <c r="I12">
+        <v>1080</v>
+      </c>
+      <c r="J12">
+        <v>1095</v>
+      </c>
+      <c r="K12">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13">
+        <v>1154</v>
+      </c>
+      <c r="H13">
+        <v>1243</v>
+      </c>
+      <c r="I13">
+        <v>1356</v>
+      </c>
+      <c r="J13">
+        <v>1358</v>
+      </c>
+      <c r="K13">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14">
+        <v>1587</v>
+      </c>
+      <c r="H14">
+        <v>1609</v>
+      </c>
+      <c r="I14">
+        <v>1638</v>
+      </c>
+      <c r="J14">
+        <v>1641</v>
+      </c>
+      <c r="K14">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15">
+        <v>5248</v>
+      </c>
+      <c r="H15">
+        <v>5224</v>
+      </c>
+      <c r="I15">
+        <v>5449</v>
+      </c>
+      <c r="J15">
+        <v>5497</v>
+      </c>
+      <c r="K15">
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16">
+        <v>1718</v>
+      </c>
+      <c r="H16">
+        <v>2678</v>
+      </c>
+      <c r="I16">
+        <v>3534</v>
+      </c>
+      <c r="J16">
+        <v>3511</v>
+      </c>
+      <c r="K16">
+        <v>3439</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17">
+        <v>2879</v>
+      </c>
+      <c r="H17">
+        <v>3792</v>
+      </c>
+      <c r="I17">
+        <v>4528</v>
+      </c>
+      <c r="J17">
+        <v>4687</v>
+      </c>
+      <c r="K17">
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18">
+        <v>13697</v>
+      </c>
+      <c r="H18">
+        <v>12899</v>
+      </c>
+      <c r="I18">
+        <v>11073</v>
+      </c>
+      <c r="J18">
+        <v>10710</v>
+      </c>
+      <c r="K18">
+        <v>10360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19">
+        <v>1009</v>
+      </c>
+      <c r="H19">
+        <v>1297</v>
+      </c>
+      <c r="I19">
+        <v>1337</v>
+      </c>
+      <c r="J19">
+        <v>1278</v>
+      </c>
+      <c r="K19">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20">
+        <v>4263</v>
+      </c>
+      <c r="H20">
+        <v>4244</v>
+      </c>
+      <c r="I20">
+        <v>4579</v>
+      </c>
+      <c r="J20">
+        <v>4539</v>
+      </c>
+      <c r="K20">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21">
+        <v>1121</v>
+      </c>
+      <c r="H21">
+        <v>1368</v>
+      </c>
+      <c r="I21">
+        <v>1755</v>
+      </c>
+      <c r="J21">
+        <v>1811</v>
+      </c>
+      <c r="K21">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
         <v>59</v>
       </c>
-      <c r="G8">
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22">
+        <v>1555</v>
+      </c>
+      <c r="H22">
+        <v>1541</v>
+      </c>
+      <c r="I22">
+        <v>1577</v>
+      </c>
+      <c r="J22">
+        <v>1514</v>
+      </c>
+      <c r="K22">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23">
+        <v>3008</v>
+      </c>
+      <c r="H23">
+        <v>3045</v>
+      </c>
+      <c r="I23">
+        <v>3707</v>
+      </c>
+      <c r="J23">
+        <v>3615</v>
+      </c>
+      <c r="K23">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24">
+        <v>1099</v>
+      </c>
+      <c r="H24">
+        <v>1232</v>
+      </c>
+      <c r="I24">
+        <v>1430</v>
+      </c>
+      <c r="J24">
+        <v>1380</v>
+      </c>
+      <c r="K24">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25">
+        <v>1078</v>
+      </c>
+      <c r="H25">
+        <v>1438</v>
+      </c>
+      <c r="I25">
+        <v>1644</v>
+      </c>
+      <c r="J25">
+        <v>1696</v>
+      </c>
+      <c r="K25">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26">
+        <v>1707</v>
+      </c>
+      <c r="H26">
+        <v>1803</v>
+      </c>
+      <c r="I26">
+        <v>2172</v>
+      </c>
+      <c r="J26">
+        <v>2117</v>
+      </c>
+      <c r="K26">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27">
+        <v>3388</v>
+      </c>
+      <c r="H27">
+        <v>3417</v>
+      </c>
+      <c r="I27">
+        <v>3500</v>
+      </c>
+      <c r="J27">
+        <v>3589</v>
+      </c>
+      <c r="K27">
+        <v>3621</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28">
+        <v>2104</v>
+      </c>
+      <c r="H28">
+        <v>2344</v>
+      </c>
+      <c r="I28">
+        <v>2382</v>
+      </c>
+      <c r="J28">
+        <v>2326</v>
+      </c>
+      <c r="K28">
+        <v>2369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29">
+        <v>6020</v>
+      </c>
+      <c r="H29">
+        <v>6332</v>
+      </c>
+      <c r="I29">
+        <v>7207</v>
+      </c>
+      <c r="J29">
+        <v>7110</v>
+      </c>
+      <c r="K29">
+        <v>7296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30">
+        <v>5867</v>
+      </c>
+      <c r="H30">
+        <v>8119</v>
+      </c>
+      <c r="I30">
+        <v>11817</v>
+      </c>
+      <c r="J30">
+        <v>12156</v>
+      </c>
+      <c r="K30">
+        <v>13636</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>80</v>
       </c>
-      <c r="H8">
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31">
+        <v>53593</v>
+      </c>
+      <c r="H31">
+        <v>39133</v>
+      </c>
+      <c r="I31">
+        <v>37099</v>
+      </c>
+      <c r="J31">
+        <v>36197</v>
+      </c>
+      <c r="K31">
+        <v>38777</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32">
+        <v>18101</v>
+      </c>
+      <c r="H32">
+        <v>13551</v>
+      </c>
+      <c r="I32">
+        <v>16331</v>
+      </c>
+      <c r="J32">
+        <v>16712</v>
+      </c>
+      <c r="K32">
+        <v>17786</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
         <v>86</v>
       </c>
-      <c r="I8">
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33">
+        <v>3607</v>
+      </c>
+      <c r="H33">
+        <v>3148</v>
+      </c>
+      <c r="I33">
+        <v>2946</v>
+      </c>
+      <c r="J33">
+        <v>2844</v>
+      </c>
+      <c r="K33">
+        <v>2808</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34">
+        <v>3149</v>
+      </c>
+      <c r="H34">
+        <v>4618</v>
+      </c>
+      <c r="I34">
+        <v>7589</v>
+      </c>
+      <c r="J34">
+        <v>8200</v>
+      </c>
+      <c r="K34">
+        <v>8325</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35">
+        <v>8668</v>
+      </c>
+      <c r="H35">
+        <v>9416</v>
+      </c>
+      <c r="I35">
+        <v>10752</v>
+      </c>
+      <c r="J35">
+        <v>10665</v>
+      </c>
+      <c r="K35">
+        <v>10979</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36">
+        <v>6000</v>
+      </c>
+      <c r="H36">
+        <v>6332</v>
+      </c>
+      <c r="I36">
+        <v>5936</v>
+      </c>
+      <c r="J36">
+        <v>6151</v>
+      </c>
+      <c r="K36">
+        <v>7407</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37">
+        <v>1952</v>
+      </c>
+      <c r="H37">
+        <v>2691</v>
+      </c>
+      <c r="I37">
+        <v>3761</v>
+      </c>
+      <c r="J37">
+        <v>3791</v>
+      </c>
+      <c r="K37">
+        <v>4392</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38">
+        <v>41</v>
+      </c>
+      <c r="H38">
+        <v>40</v>
+      </c>
+      <c r="I38">
+        <v>41</v>
+      </c>
+      <c r="J38">
+        <v>16</v>
+      </c>
+      <c r="K38">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39">
+        <v>270</v>
+      </c>
+      <c r="H39">
+        <v>212</v>
+      </c>
+      <c r="I39">
+        <v>213</v>
+      </c>
+      <c r="J39">
+        <v>232</v>
+      </c>
+      <c r="K39">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" t="s">
+        <v>102</v>
+      </c>
+      <c r="E40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G40">
+        <v>6767</v>
+      </c>
+      <c r="H40">
+        <v>17906</v>
+      </c>
+      <c r="I40">
+        <v>25070</v>
+      </c>
+      <c r="J40">
+        <v>25637</v>
+      </c>
+      <c r="K40">
+        <v>29254</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41">
+        <v>3407</v>
+      </c>
+      <c r="H41">
+        <v>4601</v>
+      </c>
+      <c r="I41">
+        <v>6519</v>
+      </c>
+      <c r="J41">
+        <v>7068</v>
+      </c>
+      <c r="K41">
+        <v>7369</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42">
+        <v>4579</v>
+      </c>
+      <c r="H42">
+        <v>4209</v>
+      </c>
+      <c r="I42">
+        <v>4504</v>
+      </c>
+      <c r="J42">
+        <v>4673</v>
+      </c>
+      <c r="K42">
+        <v>4815</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43">
+        <v>2127</v>
+      </c>
+      <c r="H43">
+        <v>3871</v>
+      </c>
+      <c r="I43">
+        <v>7545</v>
+      </c>
+      <c r="J43">
+        <v>7777</v>
+      </c>
+      <c r="K43">
+        <v>8707</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G44">
+        <v>4154</v>
+      </c>
+      <c r="H44">
+        <v>5027</v>
+      </c>
+      <c r="I44">
+        <v>6204</v>
+      </c>
+      <c r="J44">
+        <v>6377</v>
+      </c>
+      <c r="K44">
+        <v>7035</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G45">
+        <v>1278</v>
+      </c>
+      <c r="H45">
+        <v>1100</v>
+      </c>
+      <c r="I45">
+        <v>958</v>
+      </c>
+      <c r="J45">
+        <v>992</v>
+      </c>
+      <c r="K45">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G46">
+        <v>12091</v>
+      </c>
+      <c r="H46">
+        <v>12392</v>
+      </c>
+      <c r="I46">
+        <v>13043</v>
+      </c>
+      <c r="J46">
+        <v>12542</v>
+      </c>
+      <c r="K46">
+        <v>12264</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" t="s">
+        <v>124</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G47">
+        <v>555</v>
+      </c>
+      <c r="H47">
+        <v>398</v>
+      </c>
+      <c r="I47">
+        <v>384</v>
+      </c>
+      <c r="J47">
+        <v>371</v>
+      </c>
+      <c r="K47">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G48">
+        <v>2984</v>
+      </c>
+      <c r="H48">
+        <v>3506</v>
+      </c>
+      <c r="I48">
+        <v>4630</v>
+      </c>
+      <c r="J48">
+        <v>4715</v>
+      </c>
+      <c r="K48">
+        <v>4502</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G49">
+        <v>5063</v>
+      </c>
+      <c r="H49">
+        <v>4779</v>
+      </c>
+      <c r="I49">
+        <v>5410</v>
+      </c>
+      <c r="J49">
+        <v>5338</v>
+      </c>
+      <c r="K49">
+        <v>5875</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" t="s">
+        <v>129</v>
+      </c>
+      <c r="D50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" t="s">
+        <v>130</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G50">
+        <v>4073</v>
+      </c>
+      <c r="H50">
+        <v>2986</v>
+      </c>
+      <c r="I50">
+        <v>4219</v>
+      </c>
+      <c r="J50">
+        <v>4104</v>
+      </c>
+      <c r="K50">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B51" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G51">
+        <v>2160</v>
+      </c>
+      <c r="H51">
+        <v>3276</v>
+      </c>
+      <c r="I51">
+        <v>5204</v>
+      </c>
+      <c r="J51">
+        <v>6039</v>
+      </c>
+      <c r="K51">
+        <v>8267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" t="s">
+        <v>130</v>
+      </c>
+      <c r="E52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G52">
+        <v>56</v>
+      </c>
+      <c r="H52">
         <v>68</v>
       </c>
-      <c r="J8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9">
-        <v>1572</v>
-      </c>
-      <c r="G9">
-        <v>1385</v>
-      </c>
-      <c r="H9">
-        <v>1096</v>
-      </c>
-      <c r="I9">
-        <v>1052</v>
-      </c>
-      <c r="J9">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="I52">
+        <v>79</v>
+      </c>
+      <c r="J52">
+        <v>100</v>
+      </c>
+      <c r="K52">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" t="s">
+        <v>130</v>
+      </c>
+      <c r="D53" t="s">
+        <v>130</v>
+      </c>
+      <c r="E53" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G53">
+        <v>1251</v>
+      </c>
+      <c r="H53">
+        <v>2059</v>
+      </c>
+      <c r="I53">
+        <v>2586</v>
+      </c>
+      <c r="J53">
+        <v>2802</v>
+      </c>
+      <c r="K53">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54" t="s">
+        <v>130</v>
+      </c>
+      <c r="D54" t="s">
+        <v>130</v>
+      </c>
+      <c r="E54" t="s">
+        <v>130</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54">
+        <v>1745</v>
+      </c>
+      <c r="H54">
+        <v>1642</v>
+      </c>
+      <c r="I54">
+        <v>2205</v>
+      </c>
+      <c r="J54">
+        <v>2155</v>
+      </c>
+      <c r="K54">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" t="s">
+        <v>141</v>
+      </c>
+      <c r="E55" t="s">
+        <v>130</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G55">
+        <v>3113</v>
+      </c>
+      <c r="H55">
+        <v>3805</v>
+      </c>
+      <c r="I55">
+        <v>4423</v>
+      </c>
+      <c r="J55">
+        <v>4343</v>
+      </c>
+      <c r="K55">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56" t="s">
+        <v>144</v>
+      </c>
+      <c r="E56" t="s">
+        <v>130</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G56">
+        <v>2151</v>
+      </c>
+      <c r="H56">
+        <v>1961</v>
+      </c>
+      <c r="I56">
+        <v>1967</v>
+      </c>
+      <c r="J56">
+        <v>1849</v>
+      </c>
+      <c r="K56">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
+      </c>
+      <c r="D57" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G57">
+        <v>209</v>
+      </c>
+      <c r="H57">
+        <v>291</v>
+      </c>
+      <c r="I57">
+        <v>250</v>
+      </c>
+      <c r="J57">
+        <v>236</v>
+      </c>
+      <c r="K57">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G58">
+        <v>1169</v>
+      </c>
+      <c r="H58">
+        <v>870</v>
+      </c>
+      <c r="I58">
+        <v>718</v>
+      </c>
+      <c r="J58">
+        <v>1004</v>
+      </c>
+      <c r="K58">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>337</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10">
-        <v>30857</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11">
-        <v>2150</v>
-      </c>
-      <c r="G11">
-        <v>3261</v>
-      </c>
-      <c r="H11">
-        <v>4127</v>
-      </c>
-      <c r="I11">
-        <v>4255</v>
-      </c>
-      <c r="J11">
-        <v>4636</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12">
-        <v>801</v>
-      </c>
-      <c r="G12">
-        <v>918</v>
-      </c>
-      <c r="H12">
-        <v>1080</v>
-      </c>
-      <c r="I12">
-        <v>1095</v>
-      </c>
-      <c r="J12">
-        <v>1136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13">
-        <v>1154</v>
-      </c>
-      <c r="G13">
-        <v>1243</v>
-      </c>
-      <c r="H13">
-        <v>1356</v>
-      </c>
-      <c r="I13">
-        <v>1358</v>
-      </c>
-      <c r="J13">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14">
-        <v>1587</v>
-      </c>
-      <c r="G14">
-        <v>1609</v>
-      </c>
-      <c r="H14">
-        <v>1638</v>
-      </c>
-      <c r="I14">
-        <v>1641</v>
-      </c>
-      <c r="J14">
-        <v>1732</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15">
-        <v>5248</v>
-      </c>
-      <c r="G15">
-        <v>5224</v>
-      </c>
-      <c r="H15">
-        <v>5449</v>
-      </c>
-      <c r="I15">
-        <v>5497</v>
-      </c>
-      <c r="J15">
-        <v>5520</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16">
-        <v>1718</v>
-      </c>
-      <c r="G16">
-        <v>2678</v>
-      </c>
-      <c r="H16">
-        <v>3534</v>
-      </c>
-      <c r="I16">
-        <v>3511</v>
-      </c>
-      <c r="J16">
-        <v>3439</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17">
-        <v>2879</v>
-      </c>
-      <c r="G17">
-        <v>3792</v>
-      </c>
-      <c r="H17">
-        <v>4528</v>
-      </c>
-      <c r="I17">
-        <v>4687</v>
-      </c>
-      <c r="J17">
-        <v>4637</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18">
-        <v>13697</v>
-      </c>
-      <c r="G18">
-        <v>12899</v>
-      </c>
-      <c r="H18">
-        <v>11073</v>
-      </c>
-      <c r="I18">
-        <v>10710</v>
-      </c>
-      <c r="J18">
-        <v>10360</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19">
-        <v>1009</v>
-      </c>
-      <c r="G19">
-        <v>1297</v>
-      </c>
-      <c r="H19">
-        <v>1337</v>
-      </c>
-      <c r="I19">
-        <v>1278</v>
-      </c>
-      <c r="J19">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20">
-        <v>4263</v>
-      </c>
-      <c r="G20">
-        <v>4244</v>
-      </c>
-      <c r="H20">
-        <v>4579</v>
-      </c>
-      <c r="I20">
-        <v>4539</v>
-      </c>
-      <c r="J20">
-        <v>4540</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21">
-        <v>1121</v>
-      </c>
-      <c r="G21">
-        <v>1368</v>
-      </c>
-      <c r="H21">
-        <v>1755</v>
-      </c>
-      <c r="I21">
-        <v>1811</v>
-      </c>
-      <c r="J21">
-        <v>1838</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22">
-        <v>1555</v>
-      </c>
-      <c r="G22">
-        <v>1541</v>
-      </c>
-      <c r="H22">
-        <v>1577</v>
-      </c>
-      <c r="I22">
-        <v>1514</v>
-      </c>
-      <c r="J22">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23">
-        <v>3008</v>
-      </c>
-      <c r="G23">
-        <v>3045</v>
-      </c>
-      <c r="H23">
-        <v>3707</v>
-      </c>
-      <c r="I23">
-        <v>3615</v>
-      </c>
-      <c r="J23">
-        <v>3811</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24">
-        <v>1099</v>
-      </c>
-      <c r="G24">
-        <v>1232</v>
-      </c>
-      <c r="H24">
-        <v>1430</v>
-      </c>
-      <c r="I24">
-        <v>1380</v>
-      </c>
-      <c r="J24">
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25">
-        <v>1078</v>
-      </c>
-      <c r="G25">
-        <v>1438</v>
-      </c>
-      <c r="H25">
-        <v>1644</v>
-      </c>
-      <c r="I25">
-        <v>1696</v>
-      </c>
-      <c r="J25">
-        <v>1664</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26">
-        <v>1707</v>
-      </c>
-      <c r="G26">
-        <v>1803</v>
-      </c>
-      <c r="H26">
-        <v>2172</v>
-      </c>
-      <c r="I26">
-        <v>2117</v>
-      </c>
-      <c r="J26">
-        <v>2306</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27">
-        <v>3388</v>
-      </c>
-      <c r="G27">
-        <v>3417</v>
-      </c>
-      <c r="H27">
-        <v>3500</v>
-      </c>
-      <c r="I27">
-        <v>3589</v>
-      </c>
-      <c r="J27">
-        <v>3621</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28">
-        <v>2104</v>
-      </c>
-      <c r="G28">
-        <v>2344</v>
-      </c>
-      <c r="H28">
-        <v>2382</v>
-      </c>
-      <c r="I28">
-        <v>2326</v>
-      </c>
-      <c r="J28">
-        <v>2369</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29">
-        <v>6020</v>
-      </c>
-      <c r="G29">
-        <v>6332</v>
-      </c>
-      <c r="H29">
-        <v>7207</v>
-      </c>
-      <c r="I29">
-        <v>7110</v>
-      </c>
-      <c r="J29">
-        <v>7296</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30">
-        <v>5867</v>
-      </c>
-      <c r="G30">
-        <v>8119</v>
-      </c>
-      <c r="H30">
-        <v>11817</v>
-      </c>
-      <c r="I30">
-        <v>12156</v>
-      </c>
-      <c r="J30">
-        <v>13636</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31">
-        <v>53593</v>
-      </c>
-      <c r="G31">
-        <v>39133</v>
-      </c>
-      <c r="H31">
-        <v>37099</v>
-      </c>
-      <c r="I31">
-        <v>36197</v>
-      </c>
-      <c r="J31">
-        <v>38777</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32" t="s">
-        <v>82</v>
-      </c>
-      <c r="F32">
-        <v>18101</v>
-      </c>
-      <c r="G32">
-        <v>13551</v>
-      </c>
-      <c r="H32">
-        <v>16331</v>
-      </c>
-      <c r="I32">
-        <v>16712</v>
-      </c>
-      <c r="J32">
-        <v>17786</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" t="s">
-        <v>90</v>
-      </c>
-      <c r="E33" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33">
-        <v>3607</v>
-      </c>
-      <c r="G33">
-        <v>3148</v>
-      </c>
-      <c r="H33">
-        <v>2946</v>
-      </c>
-      <c r="I33">
-        <v>2844</v>
-      </c>
-      <c r="J33">
-        <v>2808</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" t="s">
-        <v>82</v>
-      </c>
-      <c r="F34">
-        <v>3149</v>
-      </c>
-      <c r="G34">
-        <v>4618</v>
-      </c>
-      <c r="H34">
-        <v>7589</v>
-      </c>
-      <c r="I34">
-        <v>8200</v>
-      </c>
-      <c r="J34">
-        <v>8325</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35">
-        <v>8668</v>
-      </c>
-      <c r="G35">
-        <v>9416</v>
-      </c>
-      <c r="H35">
-        <v>10752</v>
-      </c>
-      <c r="I35">
-        <v>10665</v>
-      </c>
-      <c r="J35">
-        <v>10979</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36">
-        <v>6000</v>
-      </c>
-      <c r="G36">
-        <v>6332</v>
-      </c>
-      <c r="H36">
-        <v>5936</v>
-      </c>
-      <c r="I36">
-        <v>6151</v>
-      </c>
-      <c r="J36">
-        <v>7407</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" t="s">
-        <v>98</v>
-      </c>
-      <c r="F37">
-        <v>1952</v>
-      </c>
-      <c r="G37">
-        <v>2691</v>
-      </c>
-      <c r="H37">
-        <v>3761</v>
-      </c>
-      <c r="I37">
-        <v>3791</v>
-      </c>
-      <c r="J37">
-        <v>4392</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>101</v>
-      </c>
-      <c r="B38" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" t="s">
-        <v>98</v>
-      </c>
-      <c r="F38">
-        <v>41</v>
-      </c>
-      <c r="G38">
-        <v>40</v>
-      </c>
-      <c r="H38">
-        <v>41</v>
-      </c>
-      <c r="I38">
-        <v>16</v>
-      </c>
-      <c r="J38">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>103</v>
-      </c>
-      <c r="B39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" t="s">
-        <v>105</v>
-      </c>
-      <c r="E39" t="s">
-        <v>98</v>
-      </c>
-      <c r="F39">
-        <v>270</v>
-      </c>
-      <c r="G39">
-        <v>212</v>
-      </c>
-      <c r="H39">
-        <v>213</v>
-      </c>
-      <c r="I39">
-        <v>232</v>
-      </c>
-      <c r="J39">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B40" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" t="s">
-        <v>105</v>
-      </c>
-      <c r="E40" t="s">
-        <v>98</v>
-      </c>
-      <c r="F40">
-        <v>6767</v>
-      </c>
-      <c r="G40">
-        <v>17906</v>
-      </c>
-      <c r="H40">
-        <v>25070</v>
-      </c>
-      <c r="I40">
-        <v>25637</v>
-      </c>
-      <c r="J40">
-        <v>29254</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" t="s">
-        <v>105</v>
-      </c>
-      <c r="E41" t="s">
-        <v>98</v>
-      </c>
-      <c r="F41">
-        <v>3407</v>
-      </c>
-      <c r="G41">
-        <v>4601</v>
-      </c>
-      <c r="H41">
-        <v>6519</v>
-      </c>
-      <c r="I41">
-        <v>7068</v>
-      </c>
-      <c r="J41">
-        <v>7369</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" t="s">
-        <v>112</v>
-      </c>
-      <c r="E42" t="s">
-        <v>27</v>
-      </c>
-      <c r="F42">
-        <v>4579</v>
-      </c>
-      <c r="G42">
-        <v>4209</v>
-      </c>
-      <c r="H42">
-        <v>4504</v>
-      </c>
-      <c r="I42">
-        <v>4673</v>
-      </c>
-      <c r="J42">
-        <v>4815</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" t="s">
-        <v>114</v>
-      </c>
-      <c r="C43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D43" t="s">
-        <v>115</v>
-      </c>
-      <c r="E43" t="s">
-        <v>27</v>
-      </c>
-      <c r="F43">
-        <v>2127</v>
-      </c>
-      <c r="G43">
-        <v>3871</v>
-      </c>
-      <c r="H43">
-        <v>7545</v>
-      </c>
-      <c r="I43">
-        <v>7777</v>
-      </c>
-      <c r="J43">
-        <v>8707</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" t="s">
-        <v>118</v>
-      </c>
-      <c r="E44" t="s">
-        <v>98</v>
-      </c>
-      <c r="F44">
-        <v>4154</v>
-      </c>
-      <c r="G44">
-        <v>5027</v>
-      </c>
-      <c r="H44">
-        <v>6204</v>
-      </c>
-      <c r="I44">
-        <v>6377</v>
-      </c>
-      <c r="J44">
-        <v>7035</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>119</v>
-      </c>
-      <c r="B45" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45">
-        <v>1278</v>
-      </c>
-      <c r="G45">
-        <v>1100</v>
-      </c>
-      <c r="H45">
-        <v>958</v>
-      </c>
-      <c r="I45">
-        <v>992</v>
-      </c>
-      <c r="J45">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46">
-        <v>12091</v>
-      </c>
-      <c r="G46">
-        <v>12392</v>
-      </c>
-      <c r="H46">
-        <v>13043</v>
-      </c>
-      <c r="I46">
-        <v>12542</v>
-      </c>
-      <c r="J46">
-        <v>12264</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>123</v>
-      </c>
-      <c r="B47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" t="s">
-        <v>98</v>
-      </c>
-      <c r="D47" t="s">
-        <v>98</v>
-      </c>
-      <c r="E47" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47">
-        <v>555</v>
-      </c>
-      <c r="G47">
-        <v>398</v>
-      </c>
-      <c r="H47">
-        <v>384</v>
-      </c>
-      <c r="I47">
-        <v>371</v>
-      </c>
-      <c r="J47">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>125</v>
-      </c>
-      <c r="B48" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" t="s">
-        <v>127</v>
-      </c>
-      <c r="D48" t="s">
-        <v>127</v>
-      </c>
-      <c r="E48" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48">
-        <v>2984</v>
-      </c>
-      <c r="G48">
-        <v>3506</v>
-      </c>
-      <c r="H48">
-        <v>4630</v>
-      </c>
-      <c r="I48">
-        <v>4715</v>
-      </c>
-      <c r="J48">
-        <v>4502</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>128</v>
-      </c>
-      <c r="B49" t="s">
-        <v>129</v>
-      </c>
-      <c r="C49" t="s">
-        <v>98</v>
-      </c>
-      <c r="D49" t="s">
-        <v>98</v>
-      </c>
-      <c r="E49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F49">
-        <v>5063</v>
-      </c>
-      <c r="G49">
-        <v>4779</v>
-      </c>
-      <c r="H49">
-        <v>5410</v>
-      </c>
-      <c r="I49">
-        <v>5338</v>
-      </c>
-      <c r="J49">
-        <v>5875</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>130</v>
-      </c>
-      <c r="B50" t="s">
-        <v>131</v>
-      </c>
-      <c r="C50" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" t="s">
-        <v>133</v>
-      </c>
-      <c r="E50" t="s">
-        <v>133</v>
-      </c>
-      <c r="F50">
-        <v>4073</v>
-      </c>
-      <c r="G50">
-        <v>2986</v>
-      </c>
-      <c r="H50">
-        <v>4219</v>
-      </c>
-      <c r="I50">
-        <v>4104</v>
-      </c>
-      <c r="J50">
-        <v>4468</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>134</v>
-      </c>
-      <c r="B51" t="s">
-        <v>135</v>
-      </c>
-      <c r="C51" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" t="s">
-        <v>133</v>
-      </c>
-      <c r="E51" t="s">
-        <v>133</v>
-      </c>
-      <c r="F51">
-        <v>2160</v>
-      </c>
-      <c r="G51">
-        <v>3276</v>
-      </c>
-      <c r="H51">
-        <v>5204</v>
-      </c>
-      <c r="I51">
-        <v>6039</v>
-      </c>
-      <c r="J51">
-        <v>8267</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>136</v>
-      </c>
-      <c r="B52" t="s">
-        <v>137</v>
-      </c>
-      <c r="C52" t="s">
-        <v>133</v>
-      </c>
-      <c r="D52" t="s">
-        <v>133</v>
-      </c>
-      <c r="E52" t="s">
-        <v>133</v>
-      </c>
-      <c r="F52">
-        <v>56</v>
-      </c>
-      <c r="G52">
-        <v>68</v>
-      </c>
-      <c r="H52">
-        <v>79</v>
-      </c>
-      <c r="I52">
-        <v>100</v>
-      </c>
-      <c r="J52">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>138</v>
-      </c>
-      <c r="B53" t="s">
-        <v>139</v>
-      </c>
-      <c r="C53" t="s">
-        <v>133</v>
-      </c>
-      <c r="D53" t="s">
-        <v>133</v>
-      </c>
-      <c r="E53" t="s">
-        <v>133</v>
-      </c>
-      <c r="F53">
-        <v>1251</v>
-      </c>
-      <c r="G53">
-        <v>2059</v>
-      </c>
-      <c r="H53">
-        <v>2586</v>
-      </c>
-      <c r="I53">
-        <v>2802</v>
-      </c>
-      <c r="J53">
-        <v>2780</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>140</v>
-      </c>
-      <c r="B54" t="s">
-        <v>141</v>
-      </c>
-      <c r="C54" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" t="s">
-        <v>133</v>
-      </c>
-      <c r="E54" t="s">
-        <v>133</v>
-      </c>
-      <c r="F54">
-        <v>1745</v>
-      </c>
-      <c r="G54">
-        <v>1642</v>
-      </c>
-      <c r="H54">
-        <v>2205</v>
-      </c>
-      <c r="I54">
-        <v>2155</v>
-      </c>
-      <c r="J54">
-        <v>2053</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>142</v>
-      </c>
-      <c r="B55" t="s">
-        <v>143</v>
-      </c>
-      <c r="C55" t="s">
-        <v>144</v>
-      </c>
-      <c r="D55" t="s">
-        <v>144</v>
-      </c>
-      <c r="E55" t="s">
-        <v>133</v>
-      </c>
-      <c r="F55">
-        <v>3113</v>
-      </c>
-      <c r="G55">
-        <v>3805</v>
-      </c>
-      <c r="H55">
-        <v>4423</v>
-      </c>
-      <c r="I55">
-        <v>4343</v>
-      </c>
-      <c r="J55">
-        <v>3992</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B56" t="s">
-        <v>146</v>
-      </c>
-      <c r="C56" t="s">
-        <v>147</v>
-      </c>
-      <c r="D56" t="s">
-        <v>147</v>
-      </c>
-      <c r="E56" t="s">
-        <v>133</v>
-      </c>
-      <c r="F56">
-        <v>2151</v>
-      </c>
-      <c r="G56">
-        <v>1961</v>
-      </c>
-      <c r="H56">
-        <v>1967</v>
-      </c>
-      <c r="I56">
-        <v>1849</v>
-      </c>
-      <c r="J56">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>148</v>
-      </c>
-      <c r="B57" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" t="s">
-        <v>133</v>
-      </c>
-      <c r="D57" t="s">
-        <v>133</v>
-      </c>
-      <c r="E57" t="s">
-        <v>133</v>
-      </c>
-      <c r="F57">
-        <v>209</v>
-      </c>
-      <c r="G57">
-        <v>291</v>
-      </c>
-      <c r="H57">
-        <v>250</v>
-      </c>
-      <c r="I57">
-        <v>236</v>
-      </c>
-      <c r="J57">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>150</v>
-      </c>
-      <c r="B58" t="s">
+    </row>
+    <row r="60" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>151</v>
       </c>
-      <c r="C58" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" t="s">
-        <v>27</v>
-      </c>
-      <c r="E58" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58">
-        <v>1169</v>
-      </c>
-      <c r="G58">
-        <v>870</v>
-      </c>
-      <c r="H58">
-        <v>718</v>
-      </c>
-      <c r="I58">
-        <v>1004</v>
-      </c>
-      <c r="J58">
-        <v>2970</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B60" t="s">
         <v>152</v>
       </c>
-      <c r="B59" t="s">
-        <v>153</v>
-      </c>
-      <c r="C59" t="s">
-        <v>27</v>
-      </c>
-      <c r="D59" t="s">
-        <v>27</v>
-      </c>
-      <c r="E59" t="s">
-        <v>27</v>
-      </c>
-      <c r="G59">
-        <v>337</v>
-      </c>
-      <c r="J59">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>154</v>
-      </c>
-      <c r="B60" t="s">
-        <v>155</v>
-      </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D60" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E60" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Cardiovascular">
-      <formula>NOT(ISERROR(SEARCH("Cardiovascular",E1)))</formula>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Cardiovascular">
+      <formula>NOT(ISERROR(SEARCH("Cardiovascular",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Injury">
+      <formula>NOT(ISERROR(SEARCH("Injury",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Other Chronic">
+      <formula>NOT(ISERROR(SEARCH("Other Chronic",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Communicable">
+      <formula>NOT(ISERROR(SEARCH("Communicable",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="Cancer">
+      <formula>NOT(ISERROR(SEARCH("Cancer",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Cardiovascular">
+      <formula>NOT(ISERROR(SEARCH("Cardiovascular",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Injury">
+      <formula>NOT(ISERROR(SEARCH("Injury",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Other Chronic">
+      <formula>NOT(ISERROR(SEARCH("Other Chronic",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Communicable">
+      <formula>NOT(ISERROR(SEARCH("Communicable",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Cancer">
+      <formula>NOT(ISERROR(SEARCH("Cancer",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3770,27 +4096,27 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" t="s">
         <v>160</v>
       </c>
-      <c r="B2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>162</v>
       </c>
-      <c r="D2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E2" t="s">
-        <v>165</v>
-      </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="13">
         <v>53436</v>
@@ -3810,7 +4136,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" s="13">
         <v>1707</v>
@@ -3830,7 +4156,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="13">
         <v>4263</v>
@@ -3850,7 +4176,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="13">
         <v>5248</v>
@@ -3870,7 +4196,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B7" s="13">
         <v>2104</v>
@@ -3890,7 +4216,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B8" s="13">
         <v>13697</v>
@@ -3910,7 +4236,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B9" s="13">
         <v>17225</v>
@@ -3930,7 +4256,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" s="13">
         <v>2879</v>
@@ -3950,7 +4276,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B11" s="13">
         <v>3008</v>
@@ -3970,7 +4296,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="13">
         <v>3305</v>
@@ -3990,7 +4316,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B13" s="13">
         <v>92985</v>
@@ -4010,7 +4336,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B14" s="13">
         <v>5867</v>
@@ -4030,7 +4356,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B15" s="13">
         <v>53593</v>
@@ -4050,7 +4376,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B16" s="13">
         <v>15424</v>
@@ -4070,7 +4396,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B17" s="13">
         <v>18101</v>
@@ -4090,7 +4416,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B18" s="13">
         <v>10884</v>
@@ -4110,7 +4436,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" s="13">
         <v>133</v>
@@ -4130,7 +4456,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B20" s="13">
         <v>10616</v>
@@ -4150,7 +4476,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B21" s="13">
         <v>135</v>
@@ -4170,7 +4496,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B22" s="13">
         <v>14758</v>
@@ -4190,7 +4516,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B23" s="13">
         <v>2151</v>
@@ -4210,7 +4536,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B24" s="13">
         <v>5421</v>
@@ -4230,7 +4556,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B25" s="13">
         <v>4073</v>
@@ -4250,7 +4576,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B26" s="13">
         <v>3113</v>
@@ -4270,7 +4596,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27" s="13">
         <v>14640</v>
@@ -4290,7 +4616,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B28" s="13">
         <v>2127</v>
@@ -4310,7 +4636,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" s="13">
         <v>3319</v>
@@ -4330,7 +4656,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B30" s="13">
         <v>4579</v>
@@ -4350,7 +4676,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B31" s="13">
         <v>2984</v>
@@ -4370,7 +4696,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B32" s="13">
         <v>1631</v>
@@ -4390,7 +4716,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B33" s="13">
         <v>41578</v>
@@ -4410,7 +4736,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B34" s="13">
         <v>6000</v>
@@ -4430,7 +4756,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B35" s="13">
         <v>4154</v>
@@ -4450,7 +4776,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B36" s="13">
         <v>10444</v>
@@ -4470,7 +4796,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B37" s="13">
         <v>20980</v>
@@ -4490,7 +4816,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B38" s="13">
         <v>228281</v>
@@ -4517,31 +4843,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401F6810-FA8E-7647-9C40-841F9AFF83D4}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="158" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="158" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="17">
+      <c r="A1" s="18">
         <v>2000</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5">
         <v>54333</v>
@@ -4552,7 +4878,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4" s="6">
         <v>92982</v>
@@ -4563,7 +4889,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="6">
         <v>4700</v>
@@ -4574,7 +4900,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B6" s="6">
         <v>14002</v>
@@ -4585,7 +4911,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="6">
         <v>31791</v>
@@ -4596,7 +4922,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="6">
         <v>31889</v>
@@ -4607,7 +4933,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B9" s="5">
         <f>SUM(B3:B8)</f>
@@ -4619,24 +4945,24 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="18">
+      <c r="A11" s="19">
         <v>2010</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="11">
         <v>57820</v>
@@ -4647,7 +4973,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="8">
         <v>78960</v>
@@ -4658,7 +4984,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" s="8">
         <v>6147</v>
@@ -4669,7 +4995,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B16" s="8">
         <v>16855</v>
@@ -4680,7 +5006,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="8">
         <v>33808</v>
@@ -4691,7 +5017,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B18" s="8">
         <v>41250</v>
@@ -4702,7 +5028,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B19" s="11">
         <f>SUM(B13:B18)</f>
@@ -4714,24 +5040,24 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="18">
+      <c r="A21" s="19">
         <v>2018</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B23" s="11">
         <v>61300</v>
@@ -4742,7 +5068,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B24" s="8">
         <v>87282</v>
@@ -4753,7 +5079,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B25" s="8">
         <v>6785</v>
@@ -4764,7 +5090,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B26" s="8">
         <v>21159</v>
@@ -4775,7 +5101,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27" s="8">
         <v>41338</v>
@@ -4786,7 +5112,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B28" s="8">
         <v>51553</v>
@@ -4797,7 +5123,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29" s="11">
         <f>SUM(B23:B28)</f>

</xml_diff>

<commit_message>
Added 2019 and 2020 to both excel and the R markdown file. Azheimer's was added to specificLevel and DisplayLevel, Stroke was grouped into "cardiovascular" for displayLevel. R Markdown description was modified to be more formal and reflective of the project's purpose.
</commit_message>
<xml_diff>
--- a/ccb_cause_to_100_year_cause.xlsx
+++ b/ccb_cause_to_100_year_cause.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C39E6D7-5BD8-4940-846D-D134374DD05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1946F0D5-2C92-2C49-9152-9E4B27D4B883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ccb_cause_to_100_year_causes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="188" r:id="rId4"/>
+    <pivotCache cacheId="230" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1431,7 +1431,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="188" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="230" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:F38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1923,15 +1923,14 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
+      <selection pane="bottomLeft" activeCell="K60" sqref="K2:K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="95.6640625" customWidth="1"/>
+    <col min="3" max="5" width="25.83203125" customWidth="1"/>
     <col min="6" max="6" width="25.83203125" style="17" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Adjustments made to specificLevel, troubleshooting, and displayLevel categories. specificLevel ccb and cdc comparison table was given difference columns and color coded based on difference size. Text indicating which charts should be included in presetable markdown sheet were included in the R markdown code notes.
</commit_message>
<xml_diff>
--- a/ccb_cause_to_100_year_cause.xlsx
+++ b/ccb_cause_to_100_year_cause.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arikhalameyzer/Desktop/CDPH/Project/Project &amp; R/120_years_of_death/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1946F0D5-2C92-2C49-9152-9E4B27D4B883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E02324B-6664-BA4C-92B2-E379089955CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ccb_cause_to_100_year_causes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="230" r:id="rId4"/>
+    <pivotCache cacheId="250" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="169">
   <si>
     <t>causeCode</t>
   </si>
@@ -537,6 +537,12 @@
   </si>
   <si>
     <t>displayLevel</t>
+  </si>
+  <si>
+    <t>Alzheimer's</t>
+  </si>
+  <si>
+    <t>Other Neurologic</t>
   </si>
 </sst>
 </file>
@@ -1431,7 +1437,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="230" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C3E43C5-97A4-B345-9628-0871C3A58B13}" name="PivotTable26" cacheId="250" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:F38" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1921,9 +1927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K60" sqref="K2:K60"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2257,10 +2263,10 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
         <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
@@ -3033,7 +3039,7 @@
         <v>84</v>
       </c>
       <c r="E32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>79</v>
@@ -3278,7 +3284,7 @@
         <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>95</v>
@@ -3307,13 +3313,13 @@
         <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
       <c r="D40" t="s">
         <v>102</v>
       </c>
       <c r="E40" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
       <c r="F40" s="17" t="s">
         <v>95</v>
@@ -3348,7 +3354,7 @@
         <v>102</v>
       </c>
       <c r="E41" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>95</v>

</xml_diff>